<commit_message>
Edit of material database
</commit_message>
<xml_diff>
--- a/laminate_calc_theory_material_data.xlsx
+++ b/laminate_calc_theory_material_data.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="58">
   <si>
     <t>Workflow&gt;</t>
   </si>
@@ -296,9 +296,6 @@
     <t>Stacking sequence of laminate</t>
   </si>
   <si>
-    <t>test3</t>
-  </si>
-  <si>
     <t>phi</t>
   </si>
   <si>
@@ -323,10 +320,47 @@
     <t>Angle</t>
   </si>
   <si>
-    <t>UD160</t>
+    <t>NA</t>
   </si>
   <si>
-    <t>NA</t>
+    <r>
+      <t>σ</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t>cL</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>σ</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t>cT</t>
+    </r>
+  </si>
+  <si>
+    <t>test_nasa</t>
+  </si>
+  <si>
+    <t>test</t>
   </si>
 </sst>
 </file>
@@ -3962,8 +3996,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="14317976" y="138367"/>
-          <a:ext cx="5068734" cy="4648465"/>
+          <a:off x="14341296" y="138367"/>
+          <a:ext cx="5079244" cy="4638612"/>
           <a:chOff x="6626087" y="4265543"/>
           <a:chExt cx="5095238" cy="4634092"/>
         </a:xfrm>
@@ -4047,8 +4081,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="10060520" y="238126"/>
-          <a:ext cx="4222699" cy="4484973"/>
+          <a:off x="10074643" y="238126"/>
+          <a:ext cx="4231896" cy="4475120"/>
           <a:chOff x="10003930" y="238126"/>
           <a:chExt cx="4191323" cy="4479370"/>
         </a:xfrm>
@@ -4526,8 +4560,8 @@
   </sheetPr>
   <dimension ref="A1:M22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4588,67 +4622,67 @@
         <v>14</v>
       </c>
       <c r="B4" s="68" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C4" s="69"/>
       <c r="D4" s="36" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="E4" s="37" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="F4" s="38" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="G4" s="39" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="H4" s="40" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="I4" s="41" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="J4" s="42" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="K4" s="43" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="L4" s="44" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="M4" s="45" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="47" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B5" s="48" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C5" s="61" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D5" s="51">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="E5" s="52">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="F5" s="53">
         <v>45</v>
       </c>
       <c r="G5" s="54">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="H5" s="55">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="I5" s="56">
-        <v>0</v>
+        <v>-45</v>
       </c>
       <c r="J5" s="57">
         <v>0</v>
@@ -4675,31 +4709,31 @@
       </c>
       <c r="D6" s="5">
         <f>HLOOKUP(D$4,Material_Database!$D$4:$N$16,2,0)</f>
-        <v>20010000</v>
+        <v>57450</v>
       </c>
       <c r="E6" s="5">
         <f>HLOOKUP(E$4,Material_Database!$D$4:$N$16,2,0)</f>
-        <v>20010000</v>
+        <v>57450</v>
       </c>
       <c r="F6" s="5">
         <f>HLOOKUP(F$4,Material_Database!$D$4:$N$16,2,0)</f>
-        <v>20010000</v>
+        <v>57450</v>
       </c>
       <c r="G6" s="5">
         <f>HLOOKUP(G$4,Material_Database!$D$4:$N$16,2,0)</f>
-        <v>20010000</v>
+        <v>57450</v>
       </c>
       <c r="H6" s="5">
         <f>HLOOKUP(H$4,Material_Database!$D$4:$N$16,2,0)</f>
-        <v>0</v>
+        <v>57450</v>
       </c>
       <c r="I6" s="5">
         <f>HLOOKUP(I$4,Material_Database!$D$4:$N$16,2,0)</f>
-        <v>0</v>
+        <v>57450</v>
       </c>
       <c r="J6" s="5">
         <f>HLOOKUP(J$4,Material_Database!$D$4:$N$16,2,0)</f>
-        <v>0</v>
+        <v>57450</v>
       </c>
       <c r="K6" s="5">
         <f>HLOOKUP(K$4,Material_Database!$D$4:$N$16,2,0)</f>
@@ -4726,31 +4760,31 @@
       </c>
       <c r="D7" s="5">
         <f>HLOOKUP(D$4,Material_Database!$D$4:$N$16,3,0)</f>
-        <v>1301000</v>
+        <v>57450</v>
       </c>
       <c r="E7" s="5">
         <f>HLOOKUP(E$4,Material_Database!$D$4:$N$16,3,0)</f>
-        <v>1301000</v>
+        <v>57450</v>
       </c>
       <c r="F7" s="5">
         <f>HLOOKUP(F$4,Material_Database!$D$4:$N$16,3,0)</f>
-        <v>1301000</v>
+        <v>57450</v>
       </c>
       <c r="G7" s="5">
         <f>HLOOKUP(G$4,Material_Database!$D$4:$N$16,3,0)</f>
-        <v>1301000</v>
+        <v>57450</v>
       </c>
       <c r="H7" s="5">
         <f>HLOOKUP(H$4,Material_Database!$D$4:$N$16,3,0)</f>
-        <v>0</v>
+        <v>57450</v>
       </c>
       <c r="I7" s="5">
         <f>HLOOKUP(I$4,Material_Database!$D$4:$N$16,3,0)</f>
-        <v>0</v>
+        <v>57450</v>
       </c>
       <c r="J7" s="5">
         <f>HLOOKUP(J$4,Material_Database!$D$4:$N$16,3,0)</f>
-        <v>0</v>
+        <v>57450</v>
       </c>
       <c r="K7" s="5">
         <f>HLOOKUP(K$4,Material_Database!$D$4:$N$16,3,0)</f>
@@ -4777,31 +4811,31 @@
       </c>
       <c r="D8" s="5">
         <f>HLOOKUP(D$4,Material_Database!$D$4:$N$16,4,0)</f>
-        <v>1001000</v>
+        <v>2630</v>
       </c>
       <c r="E8" s="5">
         <f>HLOOKUP(E$4,Material_Database!$D$4:$N$16,4,0)</f>
-        <v>1001000</v>
+        <v>2630</v>
       </c>
       <c r="F8" s="5">
         <f>HLOOKUP(F$4,Material_Database!$D$4:$N$16,4,0)</f>
-        <v>1001000</v>
+        <v>2630</v>
       </c>
       <c r="G8" s="5">
         <f>HLOOKUP(G$4,Material_Database!$D$4:$N$16,4,0)</f>
-        <v>1001000</v>
+        <v>2630</v>
       </c>
       <c r="H8" s="5">
         <f>HLOOKUP(H$4,Material_Database!$D$4:$N$16,4,0)</f>
-        <v>0</v>
+        <v>2630</v>
       </c>
       <c r="I8" s="5">
         <f>HLOOKUP(I$4,Material_Database!$D$4:$N$16,4,0)</f>
-        <v>0</v>
+        <v>2630</v>
       </c>
       <c r="J8" s="5">
         <f>HLOOKUP(J$4,Material_Database!$D$4:$N$16,4,0)</f>
-        <v>0</v>
+        <v>2630</v>
       </c>
       <c r="K8" s="5">
         <f>HLOOKUP(K$4,Material_Database!$D$4:$N$16,4,0)</f>
@@ -4828,31 +4862,31 @@
       </c>
       <c r="D9" s="5">
         <f>HLOOKUP(D$4,Material_Database!$D$4:$N$16,5,0)</f>
-        <v>0.3</v>
+        <v>3.6999999999999998E-2</v>
       </c>
       <c r="E9" s="5">
         <f>HLOOKUP(E$4,Material_Database!$D$4:$N$16,5,0)</f>
-        <v>0.3</v>
+        <v>3.6999999999999998E-2</v>
       </c>
       <c r="F9" s="5">
         <f>HLOOKUP(F$4,Material_Database!$D$4:$N$16,5,0)</f>
-        <v>0.3</v>
+        <v>3.6999999999999998E-2</v>
       </c>
       <c r="G9" s="5">
         <f>HLOOKUP(G$4,Material_Database!$D$4:$N$16,5,0)</f>
-        <v>0.3</v>
+        <v>3.6999999999999998E-2</v>
       </c>
       <c r="H9" s="5">
         <f>HLOOKUP(H$4,Material_Database!$D$4:$N$16,5,0)</f>
-        <v>0</v>
+        <v>3.6999999999999998E-2</v>
       </c>
       <c r="I9" s="5">
         <f>HLOOKUP(I$4,Material_Database!$D$4:$N$16,5,0)</f>
-        <v>0</v>
+        <v>3.6999999999999998E-2</v>
       </c>
       <c r="J9" s="5">
         <f>HLOOKUP(J$4,Material_Database!$D$4:$N$16,5,0)</f>
-        <v>0</v>
+        <v>3.6999999999999998E-2</v>
       </c>
       <c r="K9" s="5">
         <f>HLOOKUP(K$4,Material_Database!$D$4:$N$16,5,0)</f>
@@ -4879,31 +4913,31 @@
       </c>
       <c r="D10" s="5">
         <f>HLOOKUP(D$4,Material_Database!$D$4:$N$16,6,0)</f>
-        <v>14</v>
+        <v>700</v>
       </c>
       <c r="E10" s="5">
         <f>HLOOKUP(E$4,Material_Database!$D$4:$N$16,6,0)</f>
-        <v>14</v>
+        <v>700</v>
       </c>
       <c r="F10" s="5">
         <f>HLOOKUP(F$4,Material_Database!$D$4:$N$16,6,0)</f>
-        <v>14</v>
+        <v>700</v>
       </c>
       <c r="G10" s="5">
         <f>HLOOKUP(G$4,Material_Database!$D$4:$N$16,6,0)</f>
-        <v>14</v>
+        <v>700</v>
       </c>
       <c r="H10" s="5">
         <f>HLOOKUP(H$4,Material_Database!$D$4:$N$16,6,0)</f>
-        <v>0</v>
+        <v>700</v>
       </c>
       <c r="I10" s="5">
         <f>HLOOKUP(I$4,Material_Database!$D$4:$N$16,6,0)</f>
-        <v>0</v>
+        <v>700</v>
       </c>
       <c r="J10" s="5">
         <f>HLOOKUP(J$4,Material_Database!$D$4:$N$16,6,0)</f>
-        <v>0</v>
+        <v>700</v>
       </c>
       <c r="K10" s="5">
         <f>HLOOKUP(K$4,Material_Database!$D$4:$N$16,6,0)</f>
@@ -4923,38 +4957,38 @@
         <v>23</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>40</v>
+        <v>54</v>
       </c>
       <c r="C11" s="62" t="s">
         <v>31</v>
       </c>
       <c r="D11" s="5">
         <f>HLOOKUP(D$4,Material_Database!$D$4:$N$16,7,0)</f>
-        <v>15</v>
+        <v>350</v>
       </c>
       <c r="E11" s="5">
         <f>HLOOKUP(E$4,Material_Database!$D$4:$N$16,7,0)</f>
-        <v>15</v>
+        <v>350</v>
       </c>
       <c r="F11" s="5">
         <f>HLOOKUP(F$4,Material_Database!$D$4:$N$16,7,0)</f>
-        <v>15</v>
+        <v>350</v>
       </c>
       <c r="G11" s="5">
         <f>HLOOKUP(G$4,Material_Database!$D$4:$N$16,7,0)</f>
-        <v>15</v>
+        <v>350</v>
       </c>
       <c r="H11" s="5">
         <f>HLOOKUP(H$4,Material_Database!$D$4:$N$16,7,0)</f>
-        <v>0</v>
+        <v>350</v>
       </c>
       <c r="I11" s="5">
         <f>HLOOKUP(I$4,Material_Database!$D$4:$N$16,7,0)</f>
-        <v>0</v>
+        <v>350</v>
       </c>
       <c r="J11" s="5">
         <f>HLOOKUP(J$4,Material_Database!$D$4:$N$16,7,0)</f>
-        <v>0</v>
+        <v>350</v>
       </c>
       <c r="K11" s="5">
         <f>HLOOKUP(K$4,Material_Database!$D$4:$N$16,7,0)</f>
@@ -4981,31 +5015,31 @@
       </c>
       <c r="D12" s="5">
         <f>HLOOKUP(D$4,Material_Database!$D$4:$N$16,8,0)</f>
-        <v>16</v>
+        <v>700</v>
       </c>
       <c r="E12" s="5">
         <f>HLOOKUP(E$4,Material_Database!$D$4:$N$16,8,0)</f>
-        <v>16</v>
+        <v>700</v>
       </c>
       <c r="F12" s="5">
         <f>HLOOKUP(F$4,Material_Database!$D$4:$N$16,8,0)</f>
-        <v>16</v>
+        <v>700</v>
       </c>
       <c r="G12" s="5">
         <f>HLOOKUP(G$4,Material_Database!$D$4:$N$16,8,0)</f>
-        <v>16</v>
+        <v>700</v>
       </c>
       <c r="H12" s="5">
         <f>HLOOKUP(H$4,Material_Database!$D$4:$N$16,8,0)</f>
-        <v>0</v>
+        <v>700</v>
       </c>
       <c r="I12" s="5">
         <f>HLOOKUP(I$4,Material_Database!$D$4:$N$16,8,0)</f>
-        <v>0</v>
+        <v>700</v>
       </c>
       <c r="J12" s="5">
         <f>HLOOKUP(J$4,Material_Database!$D$4:$N$16,8,0)</f>
-        <v>0</v>
+        <v>700</v>
       </c>
       <c r="K12" s="5">
         <f>HLOOKUP(K$4,Material_Database!$D$4:$N$16,8,0)</f>
@@ -5025,38 +5059,38 @@
         <v>25</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>39</v>
+        <v>55</v>
       </c>
       <c r="C13" s="62" t="s">
         <v>31</v>
       </c>
       <c r="D13" s="5">
         <f>HLOOKUP(D$4,Material_Database!$D$4:$N$16,9,0)</f>
-        <v>17</v>
+        <v>350</v>
       </c>
       <c r="E13" s="5">
         <f>HLOOKUP(E$4,Material_Database!$D$4:$N$16,9,0)</f>
-        <v>17</v>
+        <v>350</v>
       </c>
       <c r="F13" s="5">
         <f>HLOOKUP(F$4,Material_Database!$D$4:$N$16,9,0)</f>
-        <v>17</v>
+        <v>350</v>
       </c>
       <c r="G13" s="5">
         <f>HLOOKUP(G$4,Material_Database!$D$4:$N$16,9,0)</f>
-        <v>17</v>
+        <v>350</v>
       </c>
       <c r="H13" s="5">
         <f>HLOOKUP(H$4,Material_Database!$D$4:$N$16,9,0)</f>
-        <v>0</v>
+        <v>350</v>
       </c>
       <c r="I13" s="5">
         <f>HLOOKUP(I$4,Material_Database!$D$4:$N$16,9,0)</f>
-        <v>0</v>
+        <v>350</v>
       </c>
       <c r="J13" s="5">
         <f>HLOOKUP(J$4,Material_Database!$D$4:$N$16,9,0)</f>
-        <v>0</v>
+        <v>350</v>
       </c>
       <c r="K13" s="5">
         <f>HLOOKUP(K$4,Material_Database!$D$4:$N$16,9,0)</f>
@@ -5083,31 +5117,31 @@
       </c>
       <c r="D14" s="5">
         <f>HLOOKUP(D$4,Material_Database!$D$4:$N$16,10,0)</f>
-        <v>18</v>
+        <v>70</v>
       </c>
       <c r="E14" s="5">
         <f>HLOOKUP(E$4,Material_Database!$D$4:$N$16,10,0)</f>
-        <v>18</v>
+        <v>70</v>
       </c>
       <c r="F14" s="5">
         <f>HLOOKUP(F$4,Material_Database!$D$4:$N$16,10,0)</f>
-        <v>18</v>
+        <v>70</v>
       </c>
       <c r="G14" s="5">
         <f>HLOOKUP(G$4,Material_Database!$D$4:$N$16,10,0)</f>
-        <v>18</v>
+        <v>70</v>
       </c>
       <c r="H14" s="5">
         <f>HLOOKUP(H$4,Material_Database!$D$4:$N$16,10,0)</f>
-        <v>0</v>
+        <v>70</v>
       </c>
       <c r="I14" s="5">
         <f>HLOOKUP(I$4,Material_Database!$D$4:$N$16,10,0)</f>
-        <v>0</v>
+        <v>70</v>
       </c>
       <c r="J14" s="5">
         <f>HLOOKUP(J$4,Material_Database!$D$4:$N$16,10,0)</f>
-        <v>0</v>
+        <v>70</v>
       </c>
       <c r="K14" s="5">
         <f>HLOOKUP(K$4,Material_Database!$D$4:$N$16,10,0)</f>
@@ -5134,31 +5168,31 @@
       </c>
       <c r="D15" s="5">
         <f>HLOOKUP(D$4,Material_Database!$D$4:$N$16,11,0)</f>
-        <v>5.0000000000000001E-3</v>
+        <v>0.22</v>
       </c>
       <c r="E15" s="5">
         <f>HLOOKUP(E$4,Material_Database!$D$4:$N$16,11,0)</f>
-        <v>5.0000000000000001E-3</v>
+        <v>0.5</v>
       </c>
       <c r="F15" s="5">
         <f>HLOOKUP(F$4,Material_Database!$D$4:$N$16,11,0)</f>
-        <v>5.0000000000000001E-3</v>
+        <v>0.22</v>
       </c>
       <c r="G15" s="5">
         <f>HLOOKUP(G$4,Material_Database!$D$4:$N$16,11,0)</f>
-        <v>5.0000000000000001E-3</v>
+        <v>0.22</v>
       </c>
       <c r="H15" s="5">
         <f>HLOOKUP(H$4,Material_Database!$D$4:$N$16,11,0)</f>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="I15" s="5">
         <f>HLOOKUP(I$4,Material_Database!$D$4:$N$16,11,0)</f>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="J15" s="5">
         <f>HLOOKUP(J$4,Material_Database!$D$4:$N$16,11,0)</f>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="K15" s="5">
         <f>HLOOKUP(K$4,Material_Database!$D$4:$N$16,11,0)</f>
@@ -5185,31 +5219,31 @@
       </c>
       <c r="D16" s="5">
         <f>HLOOKUP(D$4,Material_Database!$D$4:$N$16,12,0)</f>
-        <v>20</v>
+        <v>1460</v>
       </c>
       <c r="E16" s="5">
         <f>HLOOKUP(E$4,Material_Database!$D$4:$N$16,12,0)</f>
-        <v>20</v>
+        <v>1460</v>
       </c>
       <c r="F16" s="5">
         <f>HLOOKUP(F$4,Material_Database!$D$4:$N$16,12,0)</f>
-        <v>20</v>
+        <v>1460</v>
       </c>
       <c r="G16" s="5">
         <f>HLOOKUP(G$4,Material_Database!$D$4:$N$16,12,0)</f>
-        <v>20</v>
+        <v>1460</v>
       </c>
       <c r="H16" s="5">
         <f>HLOOKUP(H$4,Material_Database!$D$4:$N$16,12,0)</f>
-        <v>0</v>
+        <v>1460</v>
       </c>
       <c r="I16" s="5">
         <f>HLOOKUP(I$4,Material_Database!$D$4:$N$16,12,0)</f>
-        <v>0</v>
+        <v>1460</v>
       </c>
       <c r="J16" s="5">
         <f>HLOOKUP(J$4,Material_Database!$D$4:$N$16,12,0)</f>
-        <v>0</v>
+        <v>1460</v>
       </c>
       <c r="K16" s="5">
         <f>HLOOKUP(K$4,Material_Database!$D$4:$N$16,12,0)</f>
@@ -5236,31 +5270,31 @@
       </c>
       <c r="D17" s="49">
         <f>HLOOKUP(D$4,Material_Database!$D$4:$N$16,13,0)</f>
-        <v>21</v>
+        <v>321.2</v>
       </c>
       <c r="E17" s="49">
         <f>HLOOKUP(E$4,Material_Database!$D$4:$N$16,13,0)</f>
-        <v>21</v>
+        <v>321.2</v>
       </c>
       <c r="F17" s="49">
         <f>HLOOKUP(F$4,Material_Database!$D$4:$N$16,13,0)</f>
-        <v>21</v>
+        <v>321.2</v>
       </c>
       <c r="G17" s="49">
         <f>HLOOKUP(G$4,Material_Database!$D$4:$N$16,13,0)</f>
-        <v>21</v>
+        <v>321.2</v>
       </c>
       <c r="H17" s="49">
         <f>HLOOKUP(H$4,Material_Database!$D$4:$N$16,13,0)</f>
-        <v>0</v>
+        <v>321.2</v>
       </c>
       <c r="I17" s="49">
         <f>HLOOKUP(I$4,Material_Database!$D$4:$N$16,13,0)</f>
-        <v>0</v>
+        <v>321.2</v>
       </c>
       <c r="J17" s="49">
         <f>HLOOKUP(J$4,Material_Database!$D$4:$N$16,13,0)</f>
-        <v>0</v>
+        <v>321.2</v>
       </c>
       <c r="K17" s="49">
         <f>HLOOKUP(K$4,Material_Database!$D$4:$N$16,13,0)</f>
@@ -5280,11 +5314,11 @@
     </row>
     <row r="20" spans="1:13" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C20" s="2">
         <f>SUM(D17:M17)</f>
-        <v>84</v>
+        <v>2248.4</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>35</v>
@@ -5296,11 +5330,11 @@
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C22" s="2">
         <f>SUM(D15:M15)</f>
-        <v>0.02</v>
+        <v>2.66</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>33</v>
@@ -5313,7 +5347,8 @@
     <mergeCell ref="B4:C4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
@@ -5337,7 +5372,7 @@
   <dimension ref="A1:N16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5365,37 +5400,37 @@
       <c r="B4" s="20"/>
       <c r="C4" s="21"/>
       <c r="D4" s="64" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E4" s="22" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F4" s="20" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="G4" s="20" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="H4" s="20" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="I4" s="20" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="J4" s="20" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="K4" s="20" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="L4" s="20" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="M4" s="20" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="N4" s="21" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -5414,8 +5449,8 @@
       <c r="E5" s="15">
         <v>57450</v>
       </c>
-      <c r="F5" s="9">
-        <v>1</v>
+      <c r="F5" s="15">
+        <v>57450</v>
       </c>
       <c r="G5" s="9">
         <v>20010000</v>
@@ -5458,8 +5493,8 @@
       <c r="E6" s="16">
         <v>57450</v>
       </c>
-      <c r="F6" s="9">
-        <v>2</v>
+      <c r="F6" s="16">
+        <v>57450</v>
       </c>
       <c r="G6" s="9">
         <v>1301000</v>
@@ -5502,8 +5537,8 @@
       <c r="E7" s="16">
         <v>2630</v>
       </c>
-      <c r="F7" s="9">
-        <v>3</v>
+      <c r="F7" s="16">
+        <v>2630</v>
       </c>
       <c r="G7" s="9">
         <v>1001000</v>
@@ -5546,8 +5581,8 @@
       <c r="E8" s="16">
         <v>3.6999999999999998E-2</v>
       </c>
-      <c r="F8" s="9">
-        <v>4</v>
+      <c r="F8" s="16">
+        <v>3.6999999999999998E-2</v>
       </c>
       <c r="G8" s="9">
         <v>0.3</v>
@@ -5590,8 +5625,8 @@
       <c r="E9" s="16">
         <v>700</v>
       </c>
-      <c r="F9" s="9">
-        <v>5</v>
+      <c r="F9" s="16">
+        <v>700</v>
       </c>
       <c r="G9" s="9">
         <v>14</v>
@@ -5634,8 +5669,8 @@
       <c r="E10" s="16">
         <v>350</v>
       </c>
-      <c r="F10" s="9">
-        <v>6</v>
+      <c r="F10" s="16">
+        <v>350</v>
       </c>
       <c r="G10" s="9">
         <v>15</v>
@@ -5678,8 +5713,8 @@
       <c r="E11" s="16">
         <v>700</v>
       </c>
-      <c r="F11" s="9">
-        <v>7</v>
+      <c r="F11" s="16">
+        <v>700</v>
       </c>
       <c r="G11" s="9">
         <v>16</v>
@@ -5722,8 +5757,8 @@
       <c r="E12" s="16">
         <v>350</v>
       </c>
-      <c r="F12" s="9">
-        <v>8</v>
+      <c r="F12" s="16">
+        <v>350</v>
       </c>
       <c r="G12" s="9">
         <v>17</v>
@@ -5766,8 +5801,8 @@
       <c r="E13" s="16">
         <v>70</v>
       </c>
-      <c r="F13" s="9">
-        <v>9</v>
+      <c r="F13" s="16">
+        <v>70</v>
       </c>
       <c r="G13" s="9">
         <v>18</v>
@@ -5810,8 +5845,8 @@
       <c r="E14" s="16">
         <v>0.22</v>
       </c>
-      <c r="F14" s="9">
-        <v>10</v>
+      <c r="F14" s="16">
+        <v>0.5</v>
       </c>
       <c r="G14" s="9">
         <v>5.0000000000000001E-3</v>
@@ -5854,8 +5889,8 @@
       <c r="E15" s="16">
         <v>1460</v>
       </c>
-      <c r="F15" s="9">
-        <v>11</v>
+      <c r="F15" s="16">
+        <v>1460</v>
       </c>
       <c r="G15" s="9">
         <v>20</v>
@@ -5898,8 +5933,8 @@
       <c r="E16" s="16">
         <v>321.2</v>
       </c>
-      <c r="F16" s="9">
-        <v>12</v>
+      <c r="F16" s="16">
+        <v>321.2</v>
       </c>
       <c r="G16" s="9">
         <v>21</v>

</xml_diff>

<commit_message>
Added theory about criterions
</commit_message>
<xml_diff>
--- a/laminate_calc_theory_material_data.xlsx
+++ b/laminate_calc_theory_material_data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction,_Theory" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="60">
   <si>
     <t>Workflow&gt;</t>
   </si>
@@ -290,9 +290,6 @@
     </r>
   </si>
   <si>
-    <t>Database of material parametres, carbon cloth</t>
-  </si>
-  <si>
     <t>Stacking sequence of laminate</t>
   </si>
   <si>
@@ -362,12 +359,21 @@
   <si>
     <t>test</t>
   </si>
+  <si>
+    <t>Database of material parametres, cloth</t>
+  </si>
+  <si>
+    <t>Database of material parametres, core</t>
+  </si>
+  <si>
+    <t>Sandwich theory</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -464,6 +470,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="26"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -914,7 +928,7 @@
     <xf numFmtId="0" fontId="10" fillId="13" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1099,6 +1113,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="3" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="2" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1154,8 +1172,8 @@
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>326653</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>3277</xdr:rowOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>84920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1240,8 +1258,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="13049249" y="7754472"/>
-          <a:ext cx="9378847" cy="9849932"/>
+          <a:off x="12992099" y="7887822"/>
+          <a:ext cx="9333943" cy="9841768"/>
           <a:chOff x="12886765" y="7720855"/>
           <a:chExt cx="9273991" cy="9845130"/>
         </a:xfrm>
@@ -1439,8 +1457,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="6263290" y="0"/>
-          <a:ext cx="6753744" cy="2410649"/>
+          <a:off x="6236076" y="0"/>
+          <a:ext cx="6723808" cy="2543999"/>
           <a:chOff x="4667252" y="33616"/>
           <a:chExt cx="6674503" cy="2433061"/>
         </a:xfrm>
@@ -1549,8 +1567,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="13116484" y="56029"/>
-          <a:ext cx="6780802" cy="7471124"/>
+          <a:off x="13059334" y="56029"/>
+          <a:ext cx="6746784" cy="7604474"/>
           <a:chOff x="12909176" y="44823"/>
           <a:chExt cx="6704762" cy="7471124"/>
         </a:xfrm>
@@ -1820,8 +1838,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="6448185" y="17362714"/>
-          <a:ext cx="6410564" cy="10655710"/>
+          <a:off x="6420971" y="17487900"/>
+          <a:ext cx="6380628" cy="10655710"/>
           <a:chOff x="6163235" y="12718677"/>
           <a:chExt cx="6331323" cy="10655710"/>
         </a:xfrm>
@@ -1977,8 +1995,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="13026838" y="18105664"/>
-          <a:ext cx="6837945" cy="2360747"/>
+          <a:off x="12969688" y="18230850"/>
+          <a:ext cx="6803927" cy="2360747"/>
           <a:chOff x="12875559" y="18100862"/>
           <a:chExt cx="6761905" cy="2360747"/>
         </a:xfrm>
@@ -2129,16 +2147,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>27</xdr:col>
-      <xdr:colOff>488749</xdr:colOff>
-      <xdr:row>141</xdr:row>
-      <xdr:rowOff>18590</xdr:rowOff>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>615320</xdr:colOff>
+      <xdr:row>144</xdr:row>
+      <xdr:rowOff>184597</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>32</xdr:col>
-      <xdr:colOff>352688</xdr:colOff>
-      <xdr:row>145</xdr:row>
-      <xdr:rowOff>11194</xdr:rowOff>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>396114</xdr:colOff>
+      <xdr:row>148</xdr:row>
+      <xdr:rowOff>177201</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -2150,8 +2168,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="17021428" y="26906304"/>
-          <a:ext cx="3034403" cy="754604"/>
+          <a:off x="16617320" y="27616597"/>
+          <a:ext cx="2828794" cy="754604"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -2181,1384 +2199,6 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>185254</xdr:colOff>
-      <xdr:row>150</xdr:row>
-      <xdr:rowOff>20410</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>47523</xdr:colOff>
-      <xdr:row>168</xdr:row>
-      <xdr:rowOff>143528</xdr:rowOff>
-    </xdr:to>
-    <xdr:grpSp>
-      <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="98" name="Skupina 97"/>
-        <xdr:cNvGrpSpPr/>
-      </xdr:nvGrpSpPr>
-      <xdr:grpSpPr>
-        <a:xfrm>
-          <a:off x="7533111" y="28622624"/>
-          <a:ext cx="3536198" cy="3552118"/>
-          <a:chOff x="13139248" y="27241500"/>
-          <a:chExt cx="3519633" cy="3552118"/>
-        </a:xfrm>
-      </xdr:grpSpPr>
-      <xdr:pic>
-        <xdr:nvPicPr>
-          <xdr:cNvPr id="61" name="Obrázek 60"/>
-          <xdr:cNvPicPr>
-            <a:picLocks noChangeAspect="1"/>
-          </xdr:cNvPicPr>
-        </xdr:nvPicPr>
-        <xdr:blipFill>
-          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15"/>
-          <a:stretch>
-            <a:fillRect/>
-          </a:stretch>
-        </xdr:blipFill>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="13189324" y="29622189"/>
-            <a:ext cx="3464989" cy="1171429"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:ln>
-            <a:solidFill>
-              <a:schemeClr val="tx1"/>
-            </a:solidFill>
-          </a:ln>
-        </xdr:spPr>
-      </xdr:pic>
-      <xdr:grpSp>
-        <xdr:nvGrpSpPr>
-          <xdr:cNvPr id="97" name="Skupina 96"/>
-          <xdr:cNvGrpSpPr/>
-        </xdr:nvGrpSpPr>
-        <xdr:grpSpPr>
-          <a:xfrm>
-            <a:off x="13139248" y="27241500"/>
-            <a:ext cx="3519633" cy="2285714"/>
-            <a:chOff x="13139248" y="27241500"/>
-            <a:chExt cx="3519633" cy="2285714"/>
-          </a:xfrm>
-        </xdr:grpSpPr>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="16" name="TextovéPole 15"/>
-            <xdr:cNvSpPr txBox="1"/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="13139248" y="27439841"/>
-              <a:ext cx="777006" cy="501676"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:lnRef>
-            <a:fillRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="tx1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:r>
-                <a:rPr lang="en-GB" sz="2800" b="1">
-                  <a:solidFill>
-                    <a:srgbClr val="FF0000"/>
-                  </a:solidFill>
-                  <a:latin typeface="Centaur" panose="02030504050205020304" pitchFamily="18" charset="0"/>
-                </a:rPr>
-                <a:t>VIII</a:t>
-              </a:r>
-              <a:endParaRPr lang="cs-CZ" sz="2800" b="1">
-                <a:solidFill>
-                  <a:srgbClr val="FF0000"/>
-                </a:solidFill>
-                <a:latin typeface="Centaur" panose="02030504050205020304" pitchFamily="18" charset="0"/>
-              </a:endParaRPr>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-        <xdr:grpSp>
-          <xdr:nvGrpSpPr>
-            <xdr:cNvPr id="96" name="Skupina 95"/>
-            <xdr:cNvGrpSpPr/>
-          </xdr:nvGrpSpPr>
-          <xdr:grpSpPr>
-            <a:xfrm>
-              <a:off x="13906500" y="27241500"/>
-              <a:ext cx="2752381" cy="2285714"/>
-              <a:chOff x="13982700" y="28174950"/>
-              <a:chExt cx="2752381" cy="2285714"/>
-            </a:xfrm>
-          </xdr:grpSpPr>
-          <xdr:pic>
-            <xdr:nvPicPr>
-              <xdr:cNvPr id="93" name="Obrázek 92"/>
-              <xdr:cNvPicPr>
-                <a:picLocks noChangeAspect="1"/>
-              </xdr:cNvPicPr>
-            </xdr:nvPicPr>
-            <xdr:blipFill>
-              <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16"/>
-              <a:stretch>
-                <a:fillRect/>
-              </a:stretch>
-            </xdr:blipFill>
-            <xdr:spPr>
-              <a:xfrm>
-                <a:off x="13982700" y="28174950"/>
-                <a:ext cx="2752381" cy="2285714"/>
-              </a:xfrm>
-              <a:prstGeom prst="rect">
-                <a:avLst/>
-              </a:prstGeom>
-              <a:ln>
-                <a:solidFill>
-                  <a:schemeClr val="tx1"/>
-                </a:solidFill>
-              </a:ln>
-            </xdr:spPr>
-          </xdr:pic>
-          <xdr:sp macro="" textlink="">
-            <xdr:nvSpPr>
-              <xdr:cNvPr id="94" name="Obdélník 93"/>
-              <xdr:cNvSpPr/>
-            </xdr:nvSpPr>
-            <xdr:spPr>
-              <a:xfrm>
-                <a:off x="16149917" y="28987497"/>
-                <a:ext cx="334266" cy="267009"/>
-              </a:xfrm>
-              <a:prstGeom prst="rect">
-                <a:avLst/>
-              </a:prstGeom>
-              <a:noFill/>
-              <a:ln w="38100">
-                <a:solidFill>
-                  <a:srgbClr val="FF0000"/>
-                </a:solidFill>
-              </a:ln>
-            </xdr:spPr>
-            <xdr:style>
-              <a:lnRef idx="2">
-                <a:schemeClr val="accent1">
-                  <a:shade val="50000"/>
-                </a:schemeClr>
-              </a:lnRef>
-              <a:fillRef idx="1">
-                <a:schemeClr val="accent1"/>
-              </a:fillRef>
-              <a:effectRef idx="0">
-                <a:schemeClr val="accent1"/>
-              </a:effectRef>
-              <a:fontRef idx="minor">
-                <a:schemeClr val="lt1"/>
-              </a:fontRef>
-            </xdr:style>
-            <xdr:txBody>
-              <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr algn="l"/>
-                <a:endParaRPr lang="cs-CZ" sz="1100"/>
-              </a:p>
-            </xdr:txBody>
-          </xdr:sp>
-          <xdr:sp macro="" textlink="">
-            <xdr:nvSpPr>
-              <xdr:cNvPr id="95" name="Obdélník 94"/>
-              <xdr:cNvSpPr/>
-            </xdr:nvSpPr>
-            <xdr:spPr>
-              <a:xfrm>
-                <a:off x="15582900" y="28336875"/>
-                <a:ext cx="504825" cy="904875"/>
-              </a:xfrm>
-              <a:prstGeom prst="rect">
-                <a:avLst/>
-              </a:prstGeom>
-              <a:noFill/>
-              <a:ln w="38100">
-                <a:solidFill>
-                  <a:srgbClr val="FF0000"/>
-                </a:solidFill>
-              </a:ln>
-            </xdr:spPr>
-            <xdr:style>
-              <a:lnRef idx="2">
-                <a:schemeClr val="accent1">
-                  <a:shade val="50000"/>
-                </a:schemeClr>
-              </a:lnRef>
-              <a:fillRef idx="1">
-                <a:schemeClr val="accent1"/>
-              </a:fillRef>
-              <a:effectRef idx="0">
-                <a:schemeClr val="accent1"/>
-              </a:effectRef>
-              <a:fontRef idx="minor">
-                <a:schemeClr val="lt1"/>
-              </a:fontRef>
-            </xdr:style>
-            <xdr:txBody>
-              <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr algn="l"/>
-                <a:endParaRPr lang="cs-CZ" sz="1100"/>
-              </a:p>
-            </xdr:txBody>
-          </xdr:sp>
-        </xdr:grpSp>
-      </xdr:grpSp>
-    </xdr:grpSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>213231</xdr:colOff>
-      <xdr:row>108</xdr:row>
-      <xdr:rowOff>125344</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>42</xdr:col>
-      <xdr:colOff>517887</xdr:colOff>
-      <xdr:row>161</xdr:row>
-      <xdr:rowOff>97985</xdr:rowOff>
-    </xdr:to>
-    <xdr:grpSp>
-      <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="107" name="Skupina 106"/>
-        <xdr:cNvGrpSpPr/>
-      </xdr:nvGrpSpPr>
-      <xdr:grpSpPr>
-        <a:xfrm>
-          <a:off x="13071981" y="20726558"/>
-          <a:ext cx="13272263" cy="10069141"/>
-          <a:chOff x="13044767" y="20712950"/>
-          <a:chExt cx="13272263" cy="10069141"/>
-        </a:xfrm>
-      </xdr:grpSpPr>
-      <xdr:grpSp>
-        <xdr:nvGrpSpPr>
-          <xdr:cNvPr id="103" name="Skupina 102"/>
-          <xdr:cNvGrpSpPr/>
-        </xdr:nvGrpSpPr>
-        <xdr:grpSpPr>
-          <a:xfrm>
-            <a:off x="19520783" y="20735150"/>
-            <a:ext cx="6796247" cy="8466667"/>
-            <a:chOff x="20388238" y="18826748"/>
-            <a:chExt cx="6877890" cy="8466667"/>
-          </a:xfrm>
-        </xdr:grpSpPr>
-        <xdr:pic>
-          <xdr:nvPicPr>
-            <xdr:cNvPr id="58" name="Obrázek 57"/>
-            <xdr:cNvPicPr>
-              <a:picLocks noChangeAspect="1"/>
-            </xdr:cNvPicPr>
-          </xdr:nvPicPr>
-          <xdr:blipFill>
-            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId17"/>
-            <a:stretch>
-              <a:fillRect/>
-            </a:stretch>
-          </xdr:blipFill>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="20388238" y="18826748"/>
-              <a:ext cx="6877890" cy="8466667"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:ln>
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-            </a:ln>
-          </xdr:spPr>
-        </xdr:pic>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="86" name="Obdélník 85"/>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="20902173" y="23237503"/>
-              <a:ext cx="5089688" cy="3493582"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln w="38100">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-            </a:ln>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="2">
-              <a:schemeClr val="accent1">
-                <a:shade val="50000"/>
-              </a:schemeClr>
-            </a:lnRef>
-            <a:fillRef idx="1">
-              <a:schemeClr val="accent1"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:schemeClr val="accent1"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="lt1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr algn="l"/>
-              <a:endParaRPr lang="cs-CZ" sz="1100"/>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </xdr:grpSp>
-      <xdr:grpSp>
-        <xdr:nvGrpSpPr>
-          <xdr:cNvPr id="90" name="Skupina 89"/>
-          <xdr:cNvGrpSpPr/>
-        </xdr:nvGrpSpPr>
-        <xdr:grpSpPr>
-          <a:xfrm>
-            <a:off x="13104638" y="20712950"/>
-            <a:ext cx="6097407" cy="1899399"/>
-            <a:chOff x="13025717" y="20684376"/>
-            <a:chExt cx="6066111" cy="1899399"/>
-          </a:xfrm>
-        </xdr:grpSpPr>
-        <xdr:grpSp>
-          <xdr:nvGrpSpPr>
-            <xdr:cNvPr id="60" name="Skupina 59"/>
-            <xdr:cNvGrpSpPr/>
-          </xdr:nvGrpSpPr>
-          <xdr:grpSpPr>
-            <a:xfrm>
-              <a:off x="13025717" y="20684376"/>
-              <a:ext cx="6066111" cy="1838097"/>
-              <a:chOff x="12931588" y="20687738"/>
-              <a:chExt cx="6028571" cy="1838097"/>
-            </a:xfrm>
-          </xdr:grpSpPr>
-          <xdr:grpSp>
-            <xdr:nvGrpSpPr>
-              <xdr:cNvPr id="56" name="Skupina 55"/>
-              <xdr:cNvGrpSpPr/>
-            </xdr:nvGrpSpPr>
-            <xdr:grpSpPr>
-              <a:xfrm>
-                <a:off x="12931588" y="20687738"/>
-                <a:ext cx="6028571" cy="1838097"/>
-                <a:chOff x="12931588" y="20687738"/>
-                <a:chExt cx="6028571" cy="1838097"/>
-              </a:xfrm>
-            </xdr:grpSpPr>
-            <xdr:pic>
-              <xdr:nvPicPr>
-                <xdr:cNvPr id="52" name="Obrázek 51"/>
-                <xdr:cNvPicPr>
-                  <a:picLocks noChangeAspect="1"/>
-                </xdr:cNvPicPr>
-              </xdr:nvPicPr>
-              <xdr:blipFill>
-                <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14"/>
-                <a:stretch>
-                  <a:fillRect/>
-                </a:stretch>
-              </xdr:blipFill>
-              <xdr:spPr>
-                <a:xfrm>
-                  <a:off x="12931588" y="20697264"/>
-                  <a:ext cx="6028571" cy="1828571"/>
-                </a:xfrm>
-                <a:prstGeom prst="rect">
-                  <a:avLst/>
-                </a:prstGeom>
-                <a:ln>
-                  <a:solidFill>
-                    <a:schemeClr val="tx1"/>
-                  </a:solidFill>
-                </a:ln>
-              </xdr:spPr>
-            </xdr:pic>
-            <xdr:sp macro="" textlink="">
-              <xdr:nvSpPr>
-                <xdr:cNvPr id="54" name="TextovéPole 53"/>
-                <xdr:cNvSpPr txBox="1"/>
-              </xdr:nvSpPr>
-              <xdr:spPr>
-                <a:xfrm>
-                  <a:off x="13066060" y="20977412"/>
-                  <a:ext cx="2969558" cy="515470"/>
-                </a:xfrm>
-                <a:prstGeom prst="rect">
-                  <a:avLst/>
-                </a:prstGeom>
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:ln w="9525" cmpd="sng">
-                  <a:solidFill>
-                    <a:schemeClr val="lt1">
-                      <a:shade val="50000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                </a:ln>
-              </xdr:spPr>
-              <xdr:style>
-                <a:lnRef idx="0">
-                  <a:scrgbClr r="0" g="0" b="0"/>
-                </a:lnRef>
-                <a:fillRef idx="0">
-                  <a:scrgbClr r="0" g="0" b="0"/>
-                </a:fillRef>
-                <a:effectRef idx="0">
-                  <a:scrgbClr r="0" g="0" b="0"/>
-                </a:effectRef>
-                <a:fontRef idx="minor">
-                  <a:schemeClr val="dk1"/>
-                </a:fontRef>
-              </xdr:style>
-              <xdr:txBody>
-                <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:r>
-                    <a:rPr lang="en-GB" sz="1100"/>
-                    <a:t>z</a:t>
-                  </a:r>
-                  <a:r>
-                    <a:rPr lang="en-GB" sz="1100" baseline="0"/>
-                    <a:t> is dimension of the given plane from horizontal coordinate zero </a:t>
-                  </a:r>
-                  <a:endParaRPr lang="cs-CZ" sz="1100"/>
-                </a:p>
-              </xdr:txBody>
-            </xdr:sp>
-            <xdr:sp macro="" textlink="">
-              <xdr:nvSpPr>
-                <xdr:cNvPr id="20" name="TextovéPole 19"/>
-                <xdr:cNvSpPr txBox="1"/>
-              </xdr:nvSpPr>
-              <xdr:spPr>
-                <a:xfrm>
-                  <a:off x="16116162" y="20687738"/>
-                  <a:ext cx="660589" cy="501676"/>
-                </a:xfrm>
-                <a:prstGeom prst="rect">
-                  <a:avLst/>
-                </a:prstGeom>
-                <a:noFill/>
-              </xdr:spPr>
-              <xdr:style>
-                <a:lnRef idx="0">
-                  <a:scrgbClr r="0" g="0" b="0"/>
-                </a:lnRef>
-                <a:fillRef idx="0">
-                  <a:scrgbClr r="0" g="0" b="0"/>
-                </a:fillRef>
-                <a:effectRef idx="0">
-                  <a:scrgbClr r="0" g="0" b="0"/>
-                </a:effectRef>
-                <a:fontRef idx="minor">
-                  <a:schemeClr val="tx1"/>
-                </a:fontRef>
-              </xdr:style>
-              <xdr:txBody>
-                <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
-                  <a:spAutoFit/>
-                </a:bodyPr>
-                <a:lstStyle/>
-                <a:p>
-                  <a:r>
-                    <a:rPr lang="en-GB" sz="2800" b="1">
-                      <a:solidFill>
-                        <a:srgbClr val="FF0000"/>
-                      </a:solidFill>
-                      <a:latin typeface="Centaur" panose="02030504050205020304" pitchFamily="18" charset="0"/>
-                    </a:rPr>
-                    <a:t>VII</a:t>
-                  </a:r>
-                  <a:endParaRPr lang="cs-CZ" sz="2800" b="1">
-                    <a:solidFill>
-                      <a:srgbClr val="FF0000"/>
-                    </a:solidFill>
-                    <a:latin typeface="Centaur" panose="02030504050205020304" pitchFamily="18" charset="0"/>
-                  </a:endParaRPr>
-                </a:p>
-              </xdr:txBody>
-            </xdr:sp>
-          </xdr:grpSp>
-          <xdr:sp macro="" textlink="">
-            <xdr:nvSpPr>
-              <xdr:cNvPr id="59" name="TextovéPole 58"/>
-              <xdr:cNvSpPr txBox="1"/>
-            </xdr:nvSpPr>
-            <xdr:spPr>
-              <a:xfrm>
-                <a:off x="16002000" y="21773028"/>
-                <a:ext cx="780663" cy="501676"/>
-              </a:xfrm>
-              <a:prstGeom prst="rect">
-                <a:avLst/>
-              </a:prstGeom>
-              <a:noFill/>
-            </xdr:spPr>
-            <xdr:style>
-              <a:lnRef idx="0">
-                <a:scrgbClr r="0" g="0" b="0"/>
-              </a:lnRef>
-              <a:fillRef idx="0">
-                <a:scrgbClr r="0" g="0" b="0"/>
-              </a:fillRef>
-              <a:effectRef idx="0">
-                <a:scrgbClr r="0" g="0" b="0"/>
-              </a:effectRef>
-              <a:fontRef idx="minor">
-                <a:schemeClr val="tx1"/>
-              </a:fontRef>
-            </xdr:style>
-            <xdr:txBody>
-              <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
-                <a:noAutofit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:r>
-                  <a:rPr lang="en-GB" sz="2800" b="1">
-                    <a:solidFill>
-                      <a:srgbClr val="FF0000"/>
-                    </a:solidFill>
-                    <a:latin typeface="Centaur" panose="02030504050205020304" pitchFamily="18" charset="0"/>
-                  </a:rPr>
-                  <a:t>1)</a:t>
-                </a:r>
-                <a:endParaRPr lang="cs-CZ" sz="2800" b="1">
-                  <a:solidFill>
-                    <a:srgbClr val="FF0000"/>
-                  </a:solidFill>
-                  <a:latin typeface="Centaur" panose="02030504050205020304" pitchFamily="18" charset="0"/>
-                </a:endParaRPr>
-              </a:p>
-            </xdr:txBody>
-          </xdr:sp>
-        </xdr:grpSp>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="57" name="TextovéPole 56"/>
-            <xdr:cNvSpPr txBox="1"/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="13068301" y="21518655"/>
-              <a:ext cx="3086100" cy="1065120"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:solidFill>
-              <a:schemeClr val="lt1"/>
-            </a:solidFill>
-            <a:ln w="9525" cmpd="sng">
-              <a:solidFill>
-                <a:schemeClr val="lt1">
-                  <a:shade val="50000"/>
-                </a:schemeClr>
-              </a:solidFill>
-            </a:ln>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:lnRef>
-            <a:fillRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="dk1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:r>
-                <a:rPr lang="en-GB" sz="1100"/>
-                <a:t>1)</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="en-GB" sz="1100" baseline="0"/>
-                <a:t> calculate strain in general coor system for each ply top and bottom</a:t>
-              </a:r>
-            </a:p>
-            <a:p>
-              <a:r>
-                <a:rPr lang="en-GB" sz="1100" baseline="0"/>
-                <a:t>2)plot of strain versus thickness , plies</a:t>
-              </a:r>
-            </a:p>
-            <a:p>
-              <a:r>
-                <a:rPr lang="en-GB" sz="1100" baseline="0"/>
-                <a:t>3)transform strains into material coor system </a:t>
-              </a:r>
-            </a:p>
-            <a:p>
-              <a:r>
-                <a:rPr lang="en-GB" sz="1100" baseline="0"/>
-                <a:t>4) plot strain versus thickness, plies</a:t>
-              </a:r>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </xdr:grpSp>
-      <xdr:grpSp>
-        <xdr:nvGrpSpPr>
-          <xdr:cNvPr id="92" name="Skupina 91"/>
-          <xdr:cNvGrpSpPr/>
-        </xdr:nvGrpSpPr>
-        <xdr:grpSpPr>
-          <a:xfrm>
-            <a:off x="13220138" y="25708415"/>
-            <a:ext cx="4050712" cy="2196620"/>
-            <a:chOff x="13959167" y="22881972"/>
-            <a:chExt cx="4024377" cy="2196620"/>
-          </a:xfrm>
-        </xdr:grpSpPr>
-        <xdr:grpSp>
-          <xdr:nvGrpSpPr>
-            <xdr:cNvPr id="85" name="Skupina 84"/>
-            <xdr:cNvGrpSpPr/>
-          </xdr:nvGrpSpPr>
-          <xdr:grpSpPr>
-            <a:xfrm>
-              <a:off x="14480460" y="22881972"/>
-              <a:ext cx="3503084" cy="2196620"/>
-              <a:chOff x="13902334" y="23905289"/>
-              <a:chExt cx="3522962" cy="2196620"/>
-            </a:xfrm>
-          </xdr:grpSpPr>
-          <xdr:grpSp>
-            <xdr:nvGrpSpPr>
-              <xdr:cNvPr id="68" name="Skupina 67"/>
-              <xdr:cNvGrpSpPr/>
-            </xdr:nvGrpSpPr>
-            <xdr:grpSpPr>
-              <a:xfrm>
-                <a:off x="13902334" y="23905289"/>
-                <a:ext cx="3522962" cy="1323810"/>
-                <a:chOff x="13761529" y="24128919"/>
-                <a:chExt cx="3522962" cy="1323810"/>
-              </a:xfrm>
-            </xdr:grpSpPr>
-            <xdr:grpSp>
-              <xdr:nvGrpSpPr>
-                <xdr:cNvPr id="65" name="Skupina 64"/>
-                <xdr:cNvGrpSpPr/>
-              </xdr:nvGrpSpPr>
-              <xdr:grpSpPr>
-                <a:xfrm>
-                  <a:off x="13761529" y="24128919"/>
-                  <a:ext cx="3522962" cy="1323810"/>
-                  <a:chOff x="13717545" y="24125492"/>
-                  <a:chExt cx="3510967" cy="1323810"/>
-                </a:xfrm>
-              </xdr:grpSpPr>
-              <xdr:pic>
-                <xdr:nvPicPr>
-                  <xdr:cNvPr id="62" name="Obrázek 61"/>
-                  <xdr:cNvPicPr>
-                    <a:picLocks noChangeAspect="1"/>
-                  </xdr:cNvPicPr>
-                </xdr:nvPicPr>
-                <xdr:blipFill>
-                  <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId18"/>
-                  <a:stretch>
-                    <a:fillRect/>
-                  </a:stretch>
-                </xdr:blipFill>
-                <xdr:spPr>
-                  <a:xfrm>
-                    <a:off x="13717545" y="24125492"/>
-                    <a:ext cx="3510967" cy="1323810"/>
-                  </a:xfrm>
-                  <a:prstGeom prst="rect">
-                    <a:avLst/>
-                  </a:prstGeom>
-                  <a:ln>
-                    <a:solidFill>
-                      <a:schemeClr val="tx1"/>
-                    </a:solidFill>
-                  </a:ln>
-                </xdr:spPr>
-              </xdr:pic>
-              <xdr:sp macro="" textlink="">
-                <xdr:nvSpPr>
-                  <xdr:cNvPr id="63" name="Obdélník 62"/>
-                  <xdr:cNvSpPr/>
-                </xdr:nvSpPr>
-                <xdr:spPr>
-                  <a:xfrm>
-                    <a:off x="13945914" y="24981776"/>
-                    <a:ext cx="335018" cy="267009"/>
-                  </a:xfrm>
-                  <a:prstGeom prst="rect">
-                    <a:avLst/>
-                  </a:prstGeom>
-                  <a:noFill/>
-                  <a:ln w="38100">
-                    <a:solidFill>
-                      <a:srgbClr val="FF0000"/>
-                    </a:solidFill>
-                  </a:ln>
-                </xdr:spPr>
-                <xdr:style>
-                  <a:lnRef idx="2">
-                    <a:schemeClr val="accent1">
-                      <a:shade val="50000"/>
-                    </a:schemeClr>
-                  </a:lnRef>
-                  <a:fillRef idx="1">
-                    <a:schemeClr val="accent1"/>
-                  </a:fillRef>
-                  <a:effectRef idx="0">
-                    <a:schemeClr val="accent1"/>
-                  </a:effectRef>
-                  <a:fontRef idx="minor">
-                    <a:schemeClr val="lt1"/>
-                  </a:fontRef>
-                </xdr:style>
-                <xdr:txBody>
-                  <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-                  <a:lstStyle/>
-                  <a:p>
-                    <a:pPr algn="l"/>
-                    <a:endParaRPr lang="cs-CZ" sz="1100"/>
-                  </a:p>
-                </xdr:txBody>
-              </xdr:sp>
-              <xdr:sp macro="" textlink="">
-                <xdr:nvSpPr>
-                  <xdr:cNvPr id="64" name="Obdélník 63"/>
-                  <xdr:cNvSpPr/>
-                </xdr:nvSpPr>
-                <xdr:spPr>
-                  <a:xfrm>
-                    <a:off x="16607889" y="24959751"/>
-                    <a:ext cx="335018" cy="267009"/>
-                  </a:xfrm>
-                  <a:prstGeom prst="rect">
-                    <a:avLst/>
-                  </a:prstGeom>
-                  <a:noFill/>
-                  <a:ln w="38100">
-                    <a:solidFill>
-                      <a:srgbClr val="FF0000"/>
-                    </a:solidFill>
-                  </a:ln>
-                </xdr:spPr>
-                <xdr:style>
-                  <a:lnRef idx="2">
-                    <a:schemeClr val="accent1">
-                      <a:shade val="50000"/>
-                    </a:schemeClr>
-                  </a:lnRef>
-                  <a:fillRef idx="1">
-                    <a:schemeClr val="accent1"/>
-                  </a:fillRef>
-                  <a:effectRef idx="0">
-                    <a:schemeClr val="accent1"/>
-                  </a:effectRef>
-                  <a:fontRef idx="minor">
-                    <a:schemeClr val="lt1"/>
-                  </a:fontRef>
-                </xdr:style>
-                <xdr:txBody>
-                  <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-                  <a:lstStyle/>
-                  <a:p>
-                    <a:pPr algn="l"/>
-                    <a:endParaRPr lang="cs-CZ" sz="1100"/>
-                  </a:p>
-                </xdr:txBody>
-              </xdr:sp>
-            </xdr:grpSp>
-            <xdr:sp macro="" textlink="">
-              <xdr:nvSpPr>
-                <xdr:cNvPr id="66" name="Obdélník 65"/>
-                <xdr:cNvSpPr/>
-              </xdr:nvSpPr>
-              <xdr:spPr>
-                <a:xfrm>
-                  <a:off x="15732789" y="24982028"/>
-                  <a:ext cx="336163" cy="267009"/>
-                </a:xfrm>
-                <a:prstGeom prst="rect">
-                  <a:avLst/>
-                </a:prstGeom>
-                <a:noFill/>
-                <a:ln w="38100">
-                  <a:solidFill>
-                    <a:srgbClr val="FF0000"/>
-                  </a:solidFill>
-                </a:ln>
-              </xdr:spPr>
-              <xdr:style>
-                <a:lnRef idx="2">
-                  <a:schemeClr val="accent1">
-                    <a:shade val="50000"/>
-                  </a:schemeClr>
-                </a:lnRef>
-                <a:fillRef idx="1">
-                  <a:schemeClr val="accent1"/>
-                </a:fillRef>
-                <a:effectRef idx="0">
-                  <a:schemeClr val="accent1"/>
-                </a:effectRef>
-                <a:fontRef idx="minor">
-                  <a:schemeClr val="lt1"/>
-                </a:fontRef>
-              </xdr:style>
-              <xdr:txBody>
-                <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr algn="l"/>
-                  <a:endParaRPr lang="cs-CZ" sz="1100"/>
-                </a:p>
-              </xdr:txBody>
-            </xdr:sp>
-            <xdr:sp macro="" textlink="">
-              <xdr:nvSpPr>
-                <xdr:cNvPr id="67" name="Obdélník 66"/>
-                <xdr:cNvSpPr/>
-              </xdr:nvSpPr>
-              <xdr:spPr>
-                <a:xfrm>
-                  <a:off x="14775320" y="24985341"/>
-                  <a:ext cx="336163" cy="267009"/>
-                </a:xfrm>
-                <a:prstGeom prst="rect">
-                  <a:avLst/>
-                </a:prstGeom>
-                <a:noFill/>
-                <a:ln w="38100">
-                  <a:solidFill>
-                    <a:srgbClr val="FF0000"/>
-                  </a:solidFill>
-                </a:ln>
-              </xdr:spPr>
-              <xdr:style>
-                <a:lnRef idx="2">
-                  <a:schemeClr val="accent1">
-                    <a:shade val="50000"/>
-                  </a:schemeClr>
-                </a:lnRef>
-                <a:fillRef idx="1">
-                  <a:schemeClr val="accent1"/>
-                </a:fillRef>
-                <a:effectRef idx="0">
-                  <a:schemeClr val="accent1"/>
-                </a:effectRef>
-                <a:fontRef idx="minor">
-                  <a:schemeClr val="lt1"/>
-                </a:fontRef>
-              </xdr:style>
-              <xdr:txBody>
-                <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr algn="l"/>
-                  <a:endParaRPr lang="cs-CZ" sz="1100"/>
-                </a:p>
-              </xdr:txBody>
-            </xdr:sp>
-          </xdr:grpSp>
-          <xdr:sp macro="" textlink="">
-            <xdr:nvSpPr>
-              <xdr:cNvPr id="69" name="TextovéPole 68"/>
-              <xdr:cNvSpPr txBox="1"/>
-            </xdr:nvSpPr>
-            <xdr:spPr>
-              <a:xfrm>
-                <a:off x="14147182" y="25586439"/>
-                <a:ext cx="3001717" cy="515470"/>
-              </a:xfrm>
-              <a:prstGeom prst="rect">
-                <a:avLst/>
-              </a:prstGeom>
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:ln w="38100" cmpd="sng">
-                <a:solidFill>
-                  <a:srgbClr val="FF0000"/>
-                </a:solidFill>
-              </a:ln>
-            </xdr:spPr>
-            <xdr:style>
-              <a:lnRef idx="0">
-                <a:scrgbClr r="0" g="0" b="0"/>
-              </a:lnRef>
-              <a:fillRef idx="0">
-                <a:scrgbClr r="0" g="0" b="0"/>
-              </a:fillRef>
-              <a:effectRef idx="0">
-                <a:scrgbClr r="0" g="0" b="0"/>
-              </a:effectRef>
-              <a:fontRef idx="minor">
-                <a:schemeClr val="dk1"/>
-              </a:fontRef>
-            </xdr:style>
-            <xdr:txBody>
-              <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:r>
-                  <a:rPr lang="en-GB" sz="1100"/>
-                  <a:t>NOTE:</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="en-GB" sz="1100" baseline="0"/>
-                  <a:t> when transforming strains, the </a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="en-GB" sz="1100" b="1" u="sng" baseline="0"/>
-                  <a:t>TENSORIAN </a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="en-GB" sz="1100" baseline="0"/>
-                  <a:t>strain is used</a:t>
-                </a:r>
-                <a:endParaRPr lang="cs-CZ" sz="1100"/>
-              </a:p>
-            </xdr:txBody>
-          </xdr:sp>
-          <xdr:cxnSp macro="">
-            <xdr:nvCxnSpPr>
-              <xdr:cNvPr id="71" name="Přímá spojnice 70"/>
-              <xdr:cNvCxnSpPr>
-                <a:stCxn id="69" idx="0"/>
-                <a:endCxn id="64" idx="2"/>
-              </xdr:cNvCxnSpPr>
-            </xdr:nvCxnSpPr>
-            <xdr:spPr>
-              <a:xfrm flipV="1">
-                <a:off x="15648041" y="25006557"/>
-                <a:ext cx="1322594" cy="579882"/>
-              </a:xfrm>
-              <a:prstGeom prst="line">
-                <a:avLst/>
-              </a:prstGeom>
-              <a:ln>
-                <a:solidFill>
-                  <a:srgbClr val="FF0000"/>
-                </a:solidFill>
-              </a:ln>
-            </xdr:spPr>
-            <xdr:style>
-              <a:lnRef idx="1">
-                <a:schemeClr val="accent1"/>
-              </a:lnRef>
-              <a:fillRef idx="0">
-                <a:schemeClr val="accent1"/>
-              </a:fillRef>
-              <a:effectRef idx="0">
-                <a:schemeClr val="accent1"/>
-              </a:effectRef>
-              <a:fontRef idx="minor">
-                <a:schemeClr val="tx1"/>
-              </a:fontRef>
-            </xdr:style>
-          </xdr:cxnSp>
-          <xdr:cxnSp macro="">
-            <xdr:nvCxnSpPr>
-              <xdr:cNvPr id="72" name="Přímá spojnice 71"/>
-              <xdr:cNvCxnSpPr>
-                <a:stCxn id="69" idx="0"/>
-                <a:endCxn id="66" idx="2"/>
-              </xdr:cNvCxnSpPr>
-            </xdr:nvCxnSpPr>
-            <xdr:spPr>
-              <a:xfrm flipV="1">
-                <a:off x="15648041" y="25025407"/>
-                <a:ext cx="393635" cy="561032"/>
-              </a:xfrm>
-              <a:prstGeom prst="line">
-                <a:avLst/>
-              </a:prstGeom>
-              <a:ln>
-                <a:solidFill>
-                  <a:srgbClr val="FF0000"/>
-                </a:solidFill>
-              </a:ln>
-            </xdr:spPr>
-            <xdr:style>
-              <a:lnRef idx="1">
-                <a:schemeClr val="accent1"/>
-              </a:lnRef>
-              <a:fillRef idx="0">
-                <a:schemeClr val="accent1"/>
-              </a:fillRef>
-              <a:effectRef idx="0">
-                <a:schemeClr val="accent1"/>
-              </a:effectRef>
-              <a:fontRef idx="minor">
-                <a:schemeClr val="tx1"/>
-              </a:fontRef>
-            </xdr:style>
-          </xdr:cxnSp>
-          <xdr:cxnSp macro="">
-            <xdr:nvCxnSpPr>
-              <xdr:cNvPr id="73" name="Přímá spojnice 72"/>
-              <xdr:cNvCxnSpPr>
-                <a:stCxn id="69" idx="0"/>
-                <a:endCxn id="67" idx="2"/>
-              </xdr:cNvCxnSpPr>
-            </xdr:nvCxnSpPr>
-            <xdr:spPr>
-              <a:xfrm flipH="1" flipV="1">
-                <a:off x="15084207" y="25028720"/>
-                <a:ext cx="563834" cy="557719"/>
-              </a:xfrm>
-              <a:prstGeom prst="line">
-                <a:avLst/>
-              </a:prstGeom>
-              <a:ln>
-                <a:solidFill>
-                  <a:srgbClr val="FF0000"/>
-                </a:solidFill>
-              </a:ln>
-            </xdr:spPr>
-            <xdr:style>
-              <a:lnRef idx="1">
-                <a:schemeClr val="accent1"/>
-              </a:lnRef>
-              <a:fillRef idx="0">
-                <a:schemeClr val="accent1"/>
-              </a:fillRef>
-              <a:effectRef idx="0">
-                <a:schemeClr val="accent1"/>
-              </a:effectRef>
-              <a:fontRef idx="minor">
-                <a:schemeClr val="tx1"/>
-              </a:fontRef>
-            </xdr:style>
-          </xdr:cxnSp>
-          <xdr:cxnSp macro="">
-            <xdr:nvCxnSpPr>
-              <xdr:cNvPr id="74" name="Přímá spojnice 73"/>
-              <xdr:cNvCxnSpPr>
-                <a:stCxn id="69" idx="0"/>
-                <a:endCxn id="63" idx="2"/>
-              </xdr:cNvCxnSpPr>
-            </xdr:nvCxnSpPr>
-            <xdr:spPr>
-              <a:xfrm flipH="1" flipV="1">
-                <a:off x="14299565" y="25028582"/>
-                <a:ext cx="1348476" cy="557857"/>
-              </a:xfrm>
-              <a:prstGeom prst="line">
-                <a:avLst/>
-              </a:prstGeom>
-              <a:ln>
-                <a:solidFill>
-                  <a:srgbClr val="FF0000"/>
-                </a:solidFill>
-              </a:ln>
-            </xdr:spPr>
-            <xdr:style>
-              <a:lnRef idx="1">
-                <a:schemeClr val="accent1"/>
-              </a:lnRef>
-              <a:fillRef idx="0">
-                <a:schemeClr val="accent1"/>
-              </a:fillRef>
-              <a:effectRef idx="0">
-                <a:schemeClr val="accent1"/>
-              </a:effectRef>
-              <a:fontRef idx="minor">
-                <a:schemeClr val="tx1"/>
-              </a:fontRef>
-            </xdr:style>
-          </xdr:cxnSp>
-        </xdr:grpSp>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="91" name="TextovéPole 90"/>
-            <xdr:cNvSpPr txBox="1"/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="13959167" y="23198976"/>
-              <a:ext cx="785524" cy="501676"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:lnRef>
-            <a:fillRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="tx1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
-              <a:noAutofit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:r>
-                <a:rPr lang="en-GB" sz="2800" b="1">
-                  <a:solidFill>
-                    <a:srgbClr val="FF0000"/>
-                  </a:solidFill>
-                  <a:latin typeface="Centaur" panose="02030504050205020304" pitchFamily="18" charset="0"/>
-                </a:rPr>
-                <a:t>3)</a:t>
-              </a:r>
-              <a:endParaRPr lang="cs-CZ" sz="2800" b="1">
-                <a:solidFill>
-                  <a:srgbClr val="FF0000"/>
-                </a:solidFill>
-                <a:latin typeface="Centaur" panose="02030504050205020304" pitchFamily="18" charset="0"/>
-              </a:endParaRPr>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </xdr:grpSp>
-      <xdr:grpSp>
-        <xdr:nvGrpSpPr>
-          <xdr:cNvPr id="101" name="Skupina 100"/>
-          <xdr:cNvGrpSpPr/>
-        </xdr:nvGrpSpPr>
-        <xdr:grpSpPr>
-          <a:xfrm>
-            <a:off x="13044767" y="22791964"/>
-            <a:ext cx="5010737" cy="2590800"/>
-            <a:chOff x="14149667" y="22593300"/>
-            <a:chExt cx="4984883" cy="2590800"/>
-          </a:xfrm>
-        </xdr:grpSpPr>
-        <xdr:pic>
-          <xdr:nvPicPr>
-            <xdr:cNvPr id="99" name="Obrázek 98"/>
-            <xdr:cNvPicPr>
-              <a:picLocks noChangeAspect="1"/>
-            </xdr:cNvPicPr>
-          </xdr:nvPicPr>
-          <xdr:blipFill>
-            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId19"/>
-            <a:stretch>
-              <a:fillRect/>
-            </a:stretch>
-          </xdr:blipFill>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="14544675" y="22593300"/>
-              <a:ext cx="4589875" cy="2590800"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-          </xdr:spPr>
-        </xdr:pic>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="100" name="TextovéPole 99"/>
-            <xdr:cNvSpPr txBox="1"/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="14149667" y="23237076"/>
-              <a:ext cx="785524" cy="501676"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:lnRef>
-            <a:fillRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="tx1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
-              <a:noAutofit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:r>
-                <a:rPr lang="en-GB" sz="2800" b="1">
-                  <a:solidFill>
-                    <a:srgbClr val="FF0000"/>
-                  </a:solidFill>
-                  <a:latin typeface="Centaur" panose="02030504050205020304" pitchFamily="18" charset="0"/>
-                </a:rPr>
-                <a:t>2)</a:t>
-              </a:r>
-              <a:endParaRPr lang="cs-CZ" sz="2800" b="1">
-                <a:solidFill>
-                  <a:srgbClr val="FF0000"/>
-                </a:solidFill>
-                <a:latin typeface="Centaur" panose="02030504050205020304" pitchFamily="18" charset="0"/>
-              </a:endParaRPr>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </xdr:grpSp>
-      <xdr:grpSp>
-        <xdr:nvGrpSpPr>
-          <xdr:cNvPr id="106" name="Skupina 105"/>
-          <xdr:cNvGrpSpPr/>
-        </xdr:nvGrpSpPr>
-        <xdr:grpSpPr>
-          <a:xfrm>
-            <a:off x="13362215" y="28194000"/>
-            <a:ext cx="4818821" cy="2588091"/>
-            <a:chOff x="13158107" y="28194000"/>
-            <a:chExt cx="4818821" cy="2588091"/>
-          </a:xfrm>
-        </xdr:grpSpPr>
-        <xdr:pic>
-          <xdr:nvPicPr>
-            <xdr:cNvPr id="104" name="Obrázek 103"/>
-            <xdr:cNvPicPr>
-              <a:picLocks noChangeAspect="1"/>
-            </xdr:cNvPicPr>
-          </xdr:nvPicPr>
-          <xdr:blipFill>
-            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId20"/>
-            <a:stretch>
-              <a:fillRect/>
-            </a:stretch>
-          </xdr:blipFill>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="13158107" y="28194000"/>
-              <a:ext cx="4818821" cy="2540959"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-          </xdr:spPr>
-        </xdr:pic>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="105" name="TextovéPole 104"/>
-            <xdr:cNvSpPr txBox="1"/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="13628352" y="30280415"/>
-              <a:ext cx="790664" cy="501676"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:lnRef>
-            <a:fillRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="tx1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
-              <a:noAutofit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:r>
-                <a:rPr lang="en-GB" sz="2800" b="1">
-                  <a:solidFill>
-                    <a:srgbClr val="FF0000"/>
-                  </a:solidFill>
-                  <a:latin typeface="Centaur" panose="02030504050205020304" pitchFamily="18" charset="0"/>
-                </a:rPr>
-                <a:t>4)</a:t>
-              </a:r>
-              <a:endParaRPr lang="cs-CZ" sz="2800" b="1">
-                <a:solidFill>
-                  <a:srgbClr val="FF0000"/>
-                </a:solidFill>
-                <a:latin typeface="Centaur" panose="02030504050205020304" pitchFamily="18" charset="0"/>
-              </a:endParaRPr>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </xdr:grpSp>
-    </xdr:grpSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>212912</xdr:colOff>
       <xdr:row>13</xdr:row>
@@ -3577,8 +2217,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="6336126" y="2532531"/>
-          <a:ext cx="6389609" cy="14751740"/>
+          <a:off x="6308912" y="2665881"/>
+          <a:ext cx="6362394" cy="14743576"/>
           <a:chOff x="6163236" y="2398061"/>
           <a:chExt cx="6317571" cy="14746938"/>
         </a:xfrm>
@@ -3630,7 +2270,7 @@
                 </xdr:cNvPicPr>
               </xdr:nvPicPr>
               <xdr:blipFill rotWithShape="1">
-                <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId21"/>
+                <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15"/>
                 <a:srcRect b="14922"/>
                 <a:stretch/>
               </xdr:blipFill>
@@ -3657,7 +2297,7 @@
                 </xdr:cNvPicPr>
               </xdr:nvPicPr>
               <xdr:blipFill rotWithShape="1">
-                <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId22"/>
+                <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16"/>
                 <a:srcRect t="20744" b="121"/>
                 <a:stretch/>
               </xdr:blipFill>
@@ -3770,7 +2410,7 @@
                 </xdr:cNvPicPr>
               </xdr:nvPicPr>
               <xdr:blipFill>
-                <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId23"/>
+                <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId17"/>
                 <a:stretch>
                   <a:fillRect/>
                 </a:stretch>
@@ -3798,7 +2438,7 @@
                 </xdr:cNvPicPr>
               </xdr:nvPicPr>
               <xdr:blipFill>
-                <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId24"/>
+                <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId18"/>
                 <a:stretch>
                   <a:fillRect/>
                 </a:stretch>
@@ -3840,7 +2480,7 @@
                 </xdr:cNvPicPr>
               </xdr:nvPicPr>
               <xdr:blipFill>
-                <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId25"/>
+                <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId19"/>
                 <a:stretch>
                   <a:fillRect/>
                 </a:stretch>
@@ -3971,6 +2611,1776 @@
     </xdr:grpSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>110</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>44</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>166</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="45" name="Skupina 44"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="13544550" y="21278850"/>
+          <a:ext cx="13592175" cy="10591800"/>
+          <a:chOff x="32368671" y="12676414"/>
+          <a:chExt cx="13778593" cy="10591800"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:grpSp>
+        <xdr:nvGrpSpPr>
+          <xdr:cNvPr id="107" name="Skupina 106"/>
+          <xdr:cNvGrpSpPr/>
+        </xdr:nvGrpSpPr>
+        <xdr:grpSpPr>
+          <a:xfrm>
+            <a:off x="32614560" y="12986815"/>
+            <a:ext cx="13277706" cy="10069141"/>
+            <a:chOff x="13044767" y="20712950"/>
+            <a:chExt cx="13272263" cy="10069141"/>
+          </a:xfrm>
+        </xdr:grpSpPr>
+        <xdr:grpSp>
+          <xdr:nvGrpSpPr>
+            <xdr:cNvPr id="103" name="Skupina 102"/>
+            <xdr:cNvGrpSpPr/>
+          </xdr:nvGrpSpPr>
+          <xdr:grpSpPr>
+            <a:xfrm>
+              <a:off x="19520783" y="20735150"/>
+              <a:ext cx="6796247" cy="8466667"/>
+              <a:chOff x="20388238" y="18826748"/>
+              <a:chExt cx="6877890" cy="8466667"/>
+            </a:xfrm>
+          </xdr:grpSpPr>
+          <xdr:pic>
+            <xdr:nvPicPr>
+              <xdr:cNvPr id="58" name="Obrázek 57"/>
+              <xdr:cNvPicPr>
+                <a:picLocks noChangeAspect="1"/>
+              </xdr:cNvPicPr>
+            </xdr:nvPicPr>
+            <xdr:blipFill>
+              <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId20"/>
+              <a:stretch>
+                <a:fillRect/>
+              </a:stretch>
+            </xdr:blipFill>
+            <xdr:spPr>
+              <a:xfrm>
+                <a:off x="20388238" y="18826748"/>
+                <a:ext cx="6877890" cy="8466667"/>
+              </a:xfrm>
+              <a:prstGeom prst="rect">
+                <a:avLst/>
+              </a:prstGeom>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+            </xdr:spPr>
+          </xdr:pic>
+          <xdr:sp macro="" textlink="">
+            <xdr:nvSpPr>
+              <xdr:cNvPr id="86" name="Obdélník 85"/>
+              <xdr:cNvSpPr/>
+            </xdr:nvSpPr>
+            <xdr:spPr>
+              <a:xfrm>
+                <a:off x="20902173" y="23237503"/>
+                <a:ext cx="5089688" cy="3493582"/>
+              </a:xfrm>
+              <a:prstGeom prst="rect">
+                <a:avLst/>
+              </a:prstGeom>
+              <a:noFill/>
+              <a:ln w="38100">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+              </a:ln>
+            </xdr:spPr>
+            <xdr:style>
+              <a:lnRef idx="2">
+                <a:schemeClr val="accent1">
+                  <a:shade val="50000"/>
+                </a:schemeClr>
+              </a:lnRef>
+              <a:fillRef idx="1">
+                <a:schemeClr val="accent1"/>
+              </a:fillRef>
+              <a:effectRef idx="0">
+                <a:schemeClr val="accent1"/>
+              </a:effectRef>
+              <a:fontRef idx="minor">
+                <a:schemeClr val="lt1"/>
+              </a:fontRef>
+            </xdr:style>
+            <xdr:txBody>
+              <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr algn="l"/>
+                <a:endParaRPr lang="cs-CZ" sz="1100"/>
+              </a:p>
+            </xdr:txBody>
+          </xdr:sp>
+        </xdr:grpSp>
+        <xdr:grpSp>
+          <xdr:nvGrpSpPr>
+            <xdr:cNvPr id="90" name="Skupina 89"/>
+            <xdr:cNvGrpSpPr/>
+          </xdr:nvGrpSpPr>
+          <xdr:grpSpPr>
+            <a:xfrm>
+              <a:off x="13104638" y="20712950"/>
+              <a:ext cx="6097407" cy="1899399"/>
+              <a:chOff x="13025717" y="20684376"/>
+              <a:chExt cx="6066111" cy="1899399"/>
+            </a:xfrm>
+          </xdr:grpSpPr>
+          <xdr:grpSp>
+            <xdr:nvGrpSpPr>
+              <xdr:cNvPr id="60" name="Skupina 59"/>
+              <xdr:cNvGrpSpPr/>
+            </xdr:nvGrpSpPr>
+            <xdr:grpSpPr>
+              <a:xfrm>
+                <a:off x="13025717" y="20684376"/>
+                <a:ext cx="6066111" cy="1838097"/>
+                <a:chOff x="12931588" y="20687738"/>
+                <a:chExt cx="6028571" cy="1838097"/>
+              </a:xfrm>
+            </xdr:grpSpPr>
+            <xdr:grpSp>
+              <xdr:nvGrpSpPr>
+                <xdr:cNvPr id="56" name="Skupina 55"/>
+                <xdr:cNvGrpSpPr/>
+              </xdr:nvGrpSpPr>
+              <xdr:grpSpPr>
+                <a:xfrm>
+                  <a:off x="12931588" y="20687738"/>
+                  <a:ext cx="6028571" cy="1838097"/>
+                  <a:chOff x="12931588" y="20687738"/>
+                  <a:chExt cx="6028571" cy="1838097"/>
+                </a:xfrm>
+              </xdr:grpSpPr>
+              <xdr:pic>
+                <xdr:nvPicPr>
+                  <xdr:cNvPr id="52" name="Obrázek 51"/>
+                  <xdr:cNvPicPr>
+                    <a:picLocks noChangeAspect="1"/>
+                  </xdr:cNvPicPr>
+                </xdr:nvPicPr>
+                <xdr:blipFill>
+                  <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14"/>
+                  <a:stretch>
+                    <a:fillRect/>
+                  </a:stretch>
+                </xdr:blipFill>
+                <xdr:spPr>
+                  <a:xfrm>
+                    <a:off x="12931588" y="20697264"/>
+                    <a:ext cx="6028571" cy="1828571"/>
+                  </a:xfrm>
+                  <a:prstGeom prst="rect">
+                    <a:avLst/>
+                  </a:prstGeom>
+                  <a:ln>
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                  </a:ln>
+                </xdr:spPr>
+              </xdr:pic>
+              <xdr:sp macro="" textlink="">
+                <xdr:nvSpPr>
+                  <xdr:cNvPr id="54" name="TextovéPole 53"/>
+                  <xdr:cNvSpPr txBox="1"/>
+                </xdr:nvSpPr>
+                <xdr:spPr>
+                  <a:xfrm>
+                    <a:off x="13066060" y="20977412"/>
+                    <a:ext cx="2969558" cy="515470"/>
+                  </a:xfrm>
+                  <a:prstGeom prst="rect">
+                    <a:avLst/>
+                  </a:prstGeom>
+                  <a:solidFill>
+                    <a:schemeClr val="lt1"/>
+                  </a:solidFill>
+                  <a:ln w="9525" cmpd="sng">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:shade val="50000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                  </a:ln>
+                </xdr:spPr>
+                <xdr:style>
+                  <a:lnRef idx="0">
+                    <a:scrgbClr r="0" g="0" b="0"/>
+                  </a:lnRef>
+                  <a:fillRef idx="0">
+                    <a:scrgbClr r="0" g="0" b="0"/>
+                  </a:fillRef>
+                  <a:effectRef idx="0">
+                    <a:scrgbClr r="0" g="0" b="0"/>
+                  </a:effectRef>
+                  <a:fontRef idx="minor">
+                    <a:schemeClr val="dk1"/>
+                  </a:fontRef>
+                </xdr:style>
+                <xdr:txBody>
+                  <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-GB" sz="1100"/>
+                      <a:t>z</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-GB" sz="1100" baseline="0"/>
+                      <a:t> is dimension of the given plane from horizontal coordinate zero </a:t>
+                    </a:r>
+                    <a:endParaRPr lang="cs-CZ" sz="1100"/>
+                  </a:p>
+                </xdr:txBody>
+              </xdr:sp>
+              <xdr:sp macro="" textlink="">
+                <xdr:nvSpPr>
+                  <xdr:cNvPr id="20" name="TextovéPole 19"/>
+                  <xdr:cNvSpPr txBox="1"/>
+                </xdr:nvSpPr>
+                <xdr:spPr>
+                  <a:xfrm>
+                    <a:off x="16116162" y="20687738"/>
+                    <a:ext cx="660589" cy="501676"/>
+                  </a:xfrm>
+                  <a:prstGeom prst="rect">
+                    <a:avLst/>
+                  </a:prstGeom>
+                  <a:noFill/>
+                </xdr:spPr>
+                <xdr:style>
+                  <a:lnRef idx="0">
+                    <a:scrgbClr r="0" g="0" b="0"/>
+                  </a:lnRef>
+                  <a:fillRef idx="0">
+                    <a:scrgbClr r="0" g="0" b="0"/>
+                  </a:fillRef>
+                  <a:effectRef idx="0">
+                    <a:scrgbClr r="0" g="0" b="0"/>
+                  </a:effectRef>
+                  <a:fontRef idx="minor">
+                    <a:schemeClr val="tx1"/>
+                  </a:fontRef>
+                </xdr:style>
+                <xdr:txBody>
+                  <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+                    <a:spAutoFit/>
+                  </a:bodyPr>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-GB" sz="2800" b="1">
+                        <a:solidFill>
+                          <a:srgbClr val="FF0000"/>
+                        </a:solidFill>
+                        <a:latin typeface="Centaur" panose="02030504050205020304" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <a:t>VII</a:t>
+                    </a:r>
+                    <a:endParaRPr lang="cs-CZ" sz="2800" b="1">
+                      <a:solidFill>
+                        <a:srgbClr val="FF0000"/>
+                      </a:solidFill>
+                      <a:latin typeface="Centaur" panose="02030504050205020304" pitchFamily="18" charset="0"/>
+                    </a:endParaRPr>
+                  </a:p>
+                </xdr:txBody>
+              </xdr:sp>
+            </xdr:grpSp>
+            <xdr:sp macro="" textlink="">
+              <xdr:nvSpPr>
+                <xdr:cNvPr id="59" name="TextovéPole 58"/>
+                <xdr:cNvSpPr txBox="1"/>
+              </xdr:nvSpPr>
+              <xdr:spPr>
+                <a:xfrm>
+                  <a:off x="16002000" y="21773028"/>
+                  <a:ext cx="780663" cy="501676"/>
+                </a:xfrm>
+                <a:prstGeom prst="rect">
+                  <a:avLst/>
+                </a:prstGeom>
+                <a:noFill/>
+              </xdr:spPr>
+              <xdr:style>
+                <a:lnRef idx="0">
+                  <a:scrgbClr r="0" g="0" b="0"/>
+                </a:lnRef>
+                <a:fillRef idx="0">
+                  <a:scrgbClr r="0" g="0" b="0"/>
+                </a:fillRef>
+                <a:effectRef idx="0">
+                  <a:scrgbClr r="0" g="0" b="0"/>
+                </a:effectRef>
+                <a:fontRef idx="minor">
+                  <a:schemeClr val="tx1"/>
+                </a:fontRef>
+              </xdr:style>
+              <xdr:txBody>
+                <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+                  <a:noAutofit/>
+                </a:bodyPr>
+                <a:lstStyle/>
+                <a:p>
+                  <a:r>
+                    <a:rPr lang="en-GB" sz="2800" b="1">
+                      <a:solidFill>
+                        <a:srgbClr val="FF0000"/>
+                      </a:solidFill>
+                      <a:latin typeface="Centaur" panose="02030504050205020304" pitchFamily="18" charset="0"/>
+                    </a:rPr>
+                    <a:t>1)</a:t>
+                  </a:r>
+                  <a:endParaRPr lang="cs-CZ" sz="2800" b="1">
+                    <a:solidFill>
+                      <a:srgbClr val="FF0000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Centaur" panose="02030504050205020304" pitchFamily="18" charset="0"/>
+                  </a:endParaRPr>
+                </a:p>
+              </xdr:txBody>
+            </xdr:sp>
+          </xdr:grpSp>
+          <xdr:sp macro="" textlink="">
+            <xdr:nvSpPr>
+              <xdr:cNvPr id="57" name="TextovéPole 56"/>
+              <xdr:cNvSpPr txBox="1"/>
+            </xdr:nvSpPr>
+            <xdr:spPr>
+              <a:xfrm>
+                <a:off x="13068301" y="21518655"/>
+                <a:ext cx="3086100" cy="1065120"/>
+              </a:xfrm>
+              <a:prstGeom prst="rect">
+                <a:avLst/>
+              </a:prstGeom>
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:ln w="9525" cmpd="sng">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:shade val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+            </xdr:spPr>
+            <xdr:style>
+              <a:lnRef idx="0">
+                <a:scrgbClr r="0" g="0" b="0"/>
+              </a:lnRef>
+              <a:fillRef idx="0">
+                <a:scrgbClr r="0" g="0" b="0"/>
+              </a:fillRef>
+              <a:effectRef idx="0">
+                <a:scrgbClr r="0" g="0" b="0"/>
+              </a:effectRef>
+              <a:fontRef idx="minor">
+                <a:schemeClr val="dk1"/>
+              </a:fontRef>
+            </xdr:style>
+            <xdr:txBody>
+              <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1100"/>
+                  <a:t>1)</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1100" baseline="0"/>
+                  <a:t> calculate strain in general coor system for each ply top and bottom</a:t>
+                </a:r>
+              </a:p>
+              <a:p>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1100" baseline="0"/>
+                  <a:t>2)plot of strain versus thickness , plies</a:t>
+                </a:r>
+              </a:p>
+              <a:p>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1100" baseline="0"/>
+                  <a:t>3)transform strains into material coor system </a:t>
+                </a:r>
+              </a:p>
+              <a:p>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1100" baseline="0"/>
+                  <a:t>4) plot strain versus thickness, plies</a:t>
+                </a:r>
+              </a:p>
+            </xdr:txBody>
+          </xdr:sp>
+        </xdr:grpSp>
+        <xdr:grpSp>
+          <xdr:nvGrpSpPr>
+            <xdr:cNvPr id="92" name="Skupina 91"/>
+            <xdr:cNvGrpSpPr/>
+          </xdr:nvGrpSpPr>
+          <xdr:grpSpPr>
+            <a:xfrm>
+              <a:off x="13220138" y="25708415"/>
+              <a:ext cx="4050712" cy="2196620"/>
+              <a:chOff x="13959167" y="22881972"/>
+              <a:chExt cx="4024377" cy="2196620"/>
+            </a:xfrm>
+          </xdr:grpSpPr>
+          <xdr:grpSp>
+            <xdr:nvGrpSpPr>
+              <xdr:cNvPr id="85" name="Skupina 84"/>
+              <xdr:cNvGrpSpPr/>
+            </xdr:nvGrpSpPr>
+            <xdr:grpSpPr>
+              <a:xfrm>
+                <a:off x="14480460" y="22881972"/>
+                <a:ext cx="3503084" cy="2196620"/>
+                <a:chOff x="13902334" y="23905289"/>
+                <a:chExt cx="3522962" cy="2196620"/>
+              </a:xfrm>
+            </xdr:grpSpPr>
+            <xdr:grpSp>
+              <xdr:nvGrpSpPr>
+                <xdr:cNvPr id="68" name="Skupina 67"/>
+                <xdr:cNvGrpSpPr/>
+              </xdr:nvGrpSpPr>
+              <xdr:grpSpPr>
+                <a:xfrm>
+                  <a:off x="13902334" y="23905289"/>
+                  <a:ext cx="3522962" cy="1323810"/>
+                  <a:chOff x="13761529" y="24128919"/>
+                  <a:chExt cx="3522962" cy="1323810"/>
+                </a:xfrm>
+              </xdr:grpSpPr>
+              <xdr:grpSp>
+                <xdr:nvGrpSpPr>
+                  <xdr:cNvPr id="65" name="Skupina 64"/>
+                  <xdr:cNvGrpSpPr/>
+                </xdr:nvGrpSpPr>
+                <xdr:grpSpPr>
+                  <a:xfrm>
+                    <a:off x="13761529" y="24128919"/>
+                    <a:ext cx="3522962" cy="1323810"/>
+                    <a:chOff x="13717545" y="24125492"/>
+                    <a:chExt cx="3510967" cy="1323810"/>
+                  </a:xfrm>
+                </xdr:grpSpPr>
+                <xdr:pic>
+                  <xdr:nvPicPr>
+                    <xdr:cNvPr id="62" name="Obrázek 61"/>
+                    <xdr:cNvPicPr>
+                      <a:picLocks noChangeAspect="1"/>
+                    </xdr:cNvPicPr>
+                  </xdr:nvPicPr>
+                  <xdr:blipFill>
+                    <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId21"/>
+                    <a:stretch>
+                      <a:fillRect/>
+                    </a:stretch>
+                  </xdr:blipFill>
+                  <xdr:spPr>
+                    <a:xfrm>
+                      <a:off x="13717545" y="24125492"/>
+                      <a:ext cx="3510967" cy="1323810"/>
+                    </a:xfrm>
+                    <a:prstGeom prst="rect">
+                      <a:avLst/>
+                    </a:prstGeom>
+                    <a:ln>
+                      <a:solidFill>
+                        <a:schemeClr val="tx1"/>
+                      </a:solidFill>
+                    </a:ln>
+                  </xdr:spPr>
+                </xdr:pic>
+                <xdr:sp macro="" textlink="">
+                  <xdr:nvSpPr>
+                    <xdr:cNvPr id="63" name="Obdélník 62"/>
+                    <xdr:cNvSpPr/>
+                  </xdr:nvSpPr>
+                  <xdr:spPr>
+                    <a:xfrm>
+                      <a:off x="13945914" y="24981776"/>
+                      <a:ext cx="335018" cy="267009"/>
+                    </a:xfrm>
+                    <a:prstGeom prst="rect">
+                      <a:avLst/>
+                    </a:prstGeom>
+                    <a:noFill/>
+                    <a:ln w="38100">
+                      <a:solidFill>
+                        <a:srgbClr val="FF0000"/>
+                      </a:solidFill>
+                    </a:ln>
+                  </xdr:spPr>
+                  <xdr:style>
+                    <a:lnRef idx="2">
+                      <a:schemeClr val="accent1">
+                        <a:shade val="50000"/>
+                      </a:schemeClr>
+                    </a:lnRef>
+                    <a:fillRef idx="1">
+                      <a:schemeClr val="accent1"/>
+                    </a:fillRef>
+                    <a:effectRef idx="0">
+                      <a:schemeClr val="accent1"/>
+                    </a:effectRef>
+                    <a:fontRef idx="minor">
+                      <a:schemeClr val="lt1"/>
+                    </a:fontRef>
+                  </xdr:style>
+                  <xdr:txBody>
+                    <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+                    <a:lstStyle/>
+                    <a:p>
+                      <a:pPr algn="l"/>
+                      <a:endParaRPr lang="cs-CZ" sz="1100"/>
+                    </a:p>
+                  </xdr:txBody>
+                </xdr:sp>
+                <xdr:sp macro="" textlink="">
+                  <xdr:nvSpPr>
+                    <xdr:cNvPr id="64" name="Obdélník 63"/>
+                    <xdr:cNvSpPr/>
+                  </xdr:nvSpPr>
+                  <xdr:spPr>
+                    <a:xfrm>
+                      <a:off x="16607889" y="24959751"/>
+                      <a:ext cx="335018" cy="267009"/>
+                    </a:xfrm>
+                    <a:prstGeom prst="rect">
+                      <a:avLst/>
+                    </a:prstGeom>
+                    <a:noFill/>
+                    <a:ln w="38100">
+                      <a:solidFill>
+                        <a:srgbClr val="FF0000"/>
+                      </a:solidFill>
+                    </a:ln>
+                  </xdr:spPr>
+                  <xdr:style>
+                    <a:lnRef idx="2">
+                      <a:schemeClr val="accent1">
+                        <a:shade val="50000"/>
+                      </a:schemeClr>
+                    </a:lnRef>
+                    <a:fillRef idx="1">
+                      <a:schemeClr val="accent1"/>
+                    </a:fillRef>
+                    <a:effectRef idx="0">
+                      <a:schemeClr val="accent1"/>
+                    </a:effectRef>
+                    <a:fontRef idx="minor">
+                      <a:schemeClr val="lt1"/>
+                    </a:fontRef>
+                  </xdr:style>
+                  <xdr:txBody>
+                    <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+                    <a:lstStyle/>
+                    <a:p>
+                      <a:pPr algn="l"/>
+                      <a:endParaRPr lang="cs-CZ" sz="1100"/>
+                    </a:p>
+                  </xdr:txBody>
+                </xdr:sp>
+              </xdr:grpSp>
+              <xdr:sp macro="" textlink="">
+                <xdr:nvSpPr>
+                  <xdr:cNvPr id="66" name="Obdélník 65"/>
+                  <xdr:cNvSpPr/>
+                </xdr:nvSpPr>
+                <xdr:spPr>
+                  <a:xfrm>
+                    <a:off x="15732789" y="24982028"/>
+                    <a:ext cx="336163" cy="267009"/>
+                  </a:xfrm>
+                  <a:prstGeom prst="rect">
+                    <a:avLst/>
+                  </a:prstGeom>
+                  <a:noFill/>
+                  <a:ln w="38100">
+                    <a:solidFill>
+                      <a:srgbClr val="FF0000"/>
+                    </a:solidFill>
+                  </a:ln>
+                </xdr:spPr>
+                <xdr:style>
+                  <a:lnRef idx="2">
+                    <a:schemeClr val="accent1">
+                      <a:shade val="50000"/>
+                    </a:schemeClr>
+                  </a:lnRef>
+                  <a:fillRef idx="1">
+                    <a:schemeClr val="accent1"/>
+                  </a:fillRef>
+                  <a:effectRef idx="0">
+                    <a:schemeClr val="accent1"/>
+                  </a:effectRef>
+                  <a:fontRef idx="minor">
+                    <a:schemeClr val="lt1"/>
+                  </a:fontRef>
+                </xdr:style>
+                <xdr:txBody>
+                  <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:pPr algn="l"/>
+                    <a:endParaRPr lang="cs-CZ" sz="1100"/>
+                  </a:p>
+                </xdr:txBody>
+              </xdr:sp>
+              <xdr:sp macro="" textlink="">
+                <xdr:nvSpPr>
+                  <xdr:cNvPr id="67" name="Obdélník 66"/>
+                  <xdr:cNvSpPr/>
+                </xdr:nvSpPr>
+                <xdr:spPr>
+                  <a:xfrm>
+                    <a:off x="14775320" y="24985341"/>
+                    <a:ext cx="336163" cy="267009"/>
+                  </a:xfrm>
+                  <a:prstGeom prst="rect">
+                    <a:avLst/>
+                  </a:prstGeom>
+                  <a:noFill/>
+                  <a:ln w="38100">
+                    <a:solidFill>
+                      <a:srgbClr val="FF0000"/>
+                    </a:solidFill>
+                  </a:ln>
+                </xdr:spPr>
+                <xdr:style>
+                  <a:lnRef idx="2">
+                    <a:schemeClr val="accent1">
+                      <a:shade val="50000"/>
+                    </a:schemeClr>
+                  </a:lnRef>
+                  <a:fillRef idx="1">
+                    <a:schemeClr val="accent1"/>
+                  </a:fillRef>
+                  <a:effectRef idx="0">
+                    <a:schemeClr val="accent1"/>
+                  </a:effectRef>
+                  <a:fontRef idx="minor">
+                    <a:schemeClr val="lt1"/>
+                  </a:fontRef>
+                </xdr:style>
+                <xdr:txBody>
+                  <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:pPr algn="l"/>
+                    <a:endParaRPr lang="cs-CZ" sz="1100"/>
+                  </a:p>
+                </xdr:txBody>
+              </xdr:sp>
+            </xdr:grpSp>
+            <xdr:sp macro="" textlink="">
+              <xdr:nvSpPr>
+                <xdr:cNvPr id="69" name="TextovéPole 68"/>
+                <xdr:cNvSpPr txBox="1"/>
+              </xdr:nvSpPr>
+              <xdr:spPr>
+                <a:xfrm>
+                  <a:off x="14147182" y="25586439"/>
+                  <a:ext cx="3001717" cy="515470"/>
+                </a:xfrm>
+                <a:prstGeom prst="rect">
+                  <a:avLst/>
+                </a:prstGeom>
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:ln w="38100" cmpd="sng">
+                  <a:solidFill>
+                    <a:srgbClr val="FF0000"/>
+                  </a:solidFill>
+                </a:ln>
+              </xdr:spPr>
+              <xdr:style>
+                <a:lnRef idx="0">
+                  <a:scrgbClr r="0" g="0" b="0"/>
+                </a:lnRef>
+                <a:fillRef idx="0">
+                  <a:scrgbClr r="0" g="0" b="0"/>
+                </a:fillRef>
+                <a:effectRef idx="0">
+                  <a:scrgbClr r="0" g="0" b="0"/>
+                </a:effectRef>
+                <a:fontRef idx="minor">
+                  <a:schemeClr val="dk1"/>
+                </a:fontRef>
+              </xdr:style>
+              <xdr:txBody>
+                <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:r>
+                    <a:rPr lang="en-GB" sz="1100"/>
+                    <a:t>NOTE:</a:t>
+                  </a:r>
+                  <a:r>
+                    <a:rPr lang="en-GB" sz="1100" baseline="0"/>
+                    <a:t> when transforming strains, the </a:t>
+                  </a:r>
+                  <a:r>
+                    <a:rPr lang="en-GB" sz="1100" b="1" u="sng" baseline="0"/>
+                    <a:t>TENSORIAN </a:t>
+                  </a:r>
+                  <a:r>
+                    <a:rPr lang="en-GB" sz="1100" baseline="0"/>
+                    <a:t>strain is used</a:t>
+                  </a:r>
+                  <a:endParaRPr lang="cs-CZ" sz="1100"/>
+                </a:p>
+              </xdr:txBody>
+            </xdr:sp>
+            <xdr:cxnSp macro="">
+              <xdr:nvCxnSpPr>
+                <xdr:cNvPr id="71" name="Přímá spojnice 70"/>
+                <xdr:cNvCxnSpPr>
+                  <a:stCxn id="69" idx="0"/>
+                  <a:endCxn id="64" idx="2"/>
+                </xdr:cNvCxnSpPr>
+              </xdr:nvCxnSpPr>
+              <xdr:spPr>
+                <a:xfrm flipV="1">
+                  <a:off x="15648041" y="25006557"/>
+                  <a:ext cx="1322594" cy="579882"/>
+                </a:xfrm>
+                <a:prstGeom prst="line">
+                  <a:avLst/>
+                </a:prstGeom>
+                <a:ln>
+                  <a:solidFill>
+                    <a:srgbClr val="FF0000"/>
+                  </a:solidFill>
+                </a:ln>
+              </xdr:spPr>
+              <xdr:style>
+                <a:lnRef idx="1">
+                  <a:schemeClr val="accent1"/>
+                </a:lnRef>
+                <a:fillRef idx="0">
+                  <a:schemeClr val="accent1"/>
+                </a:fillRef>
+                <a:effectRef idx="0">
+                  <a:schemeClr val="accent1"/>
+                </a:effectRef>
+                <a:fontRef idx="minor">
+                  <a:schemeClr val="tx1"/>
+                </a:fontRef>
+              </xdr:style>
+            </xdr:cxnSp>
+            <xdr:cxnSp macro="">
+              <xdr:nvCxnSpPr>
+                <xdr:cNvPr id="72" name="Přímá spojnice 71"/>
+                <xdr:cNvCxnSpPr>
+                  <a:stCxn id="69" idx="0"/>
+                  <a:endCxn id="66" idx="2"/>
+                </xdr:cNvCxnSpPr>
+              </xdr:nvCxnSpPr>
+              <xdr:spPr>
+                <a:xfrm flipV="1">
+                  <a:off x="15648041" y="25025407"/>
+                  <a:ext cx="393635" cy="561032"/>
+                </a:xfrm>
+                <a:prstGeom prst="line">
+                  <a:avLst/>
+                </a:prstGeom>
+                <a:ln>
+                  <a:solidFill>
+                    <a:srgbClr val="FF0000"/>
+                  </a:solidFill>
+                </a:ln>
+              </xdr:spPr>
+              <xdr:style>
+                <a:lnRef idx="1">
+                  <a:schemeClr val="accent1"/>
+                </a:lnRef>
+                <a:fillRef idx="0">
+                  <a:schemeClr val="accent1"/>
+                </a:fillRef>
+                <a:effectRef idx="0">
+                  <a:schemeClr val="accent1"/>
+                </a:effectRef>
+                <a:fontRef idx="minor">
+                  <a:schemeClr val="tx1"/>
+                </a:fontRef>
+              </xdr:style>
+            </xdr:cxnSp>
+            <xdr:cxnSp macro="">
+              <xdr:nvCxnSpPr>
+                <xdr:cNvPr id="73" name="Přímá spojnice 72"/>
+                <xdr:cNvCxnSpPr>
+                  <a:stCxn id="69" idx="0"/>
+                  <a:endCxn id="67" idx="2"/>
+                </xdr:cNvCxnSpPr>
+              </xdr:nvCxnSpPr>
+              <xdr:spPr>
+                <a:xfrm flipH="1" flipV="1">
+                  <a:off x="15084207" y="25028720"/>
+                  <a:ext cx="563834" cy="557719"/>
+                </a:xfrm>
+                <a:prstGeom prst="line">
+                  <a:avLst/>
+                </a:prstGeom>
+                <a:ln>
+                  <a:solidFill>
+                    <a:srgbClr val="FF0000"/>
+                  </a:solidFill>
+                </a:ln>
+              </xdr:spPr>
+              <xdr:style>
+                <a:lnRef idx="1">
+                  <a:schemeClr val="accent1"/>
+                </a:lnRef>
+                <a:fillRef idx="0">
+                  <a:schemeClr val="accent1"/>
+                </a:fillRef>
+                <a:effectRef idx="0">
+                  <a:schemeClr val="accent1"/>
+                </a:effectRef>
+                <a:fontRef idx="minor">
+                  <a:schemeClr val="tx1"/>
+                </a:fontRef>
+              </xdr:style>
+            </xdr:cxnSp>
+            <xdr:cxnSp macro="">
+              <xdr:nvCxnSpPr>
+                <xdr:cNvPr id="74" name="Přímá spojnice 73"/>
+                <xdr:cNvCxnSpPr>
+                  <a:stCxn id="69" idx="0"/>
+                  <a:endCxn id="63" idx="2"/>
+                </xdr:cNvCxnSpPr>
+              </xdr:nvCxnSpPr>
+              <xdr:spPr>
+                <a:xfrm flipH="1" flipV="1">
+                  <a:off x="14299565" y="25028582"/>
+                  <a:ext cx="1348476" cy="557857"/>
+                </a:xfrm>
+                <a:prstGeom prst="line">
+                  <a:avLst/>
+                </a:prstGeom>
+                <a:ln>
+                  <a:solidFill>
+                    <a:srgbClr val="FF0000"/>
+                  </a:solidFill>
+                </a:ln>
+              </xdr:spPr>
+              <xdr:style>
+                <a:lnRef idx="1">
+                  <a:schemeClr val="accent1"/>
+                </a:lnRef>
+                <a:fillRef idx="0">
+                  <a:schemeClr val="accent1"/>
+                </a:fillRef>
+                <a:effectRef idx="0">
+                  <a:schemeClr val="accent1"/>
+                </a:effectRef>
+                <a:fontRef idx="minor">
+                  <a:schemeClr val="tx1"/>
+                </a:fontRef>
+              </xdr:style>
+            </xdr:cxnSp>
+          </xdr:grpSp>
+          <xdr:sp macro="" textlink="">
+            <xdr:nvSpPr>
+              <xdr:cNvPr id="91" name="TextovéPole 90"/>
+              <xdr:cNvSpPr txBox="1"/>
+            </xdr:nvSpPr>
+            <xdr:spPr>
+              <a:xfrm>
+                <a:off x="13959167" y="23198976"/>
+                <a:ext cx="785524" cy="501676"/>
+              </a:xfrm>
+              <a:prstGeom prst="rect">
+                <a:avLst/>
+              </a:prstGeom>
+              <a:noFill/>
+            </xdr:spPr>
+            <xdr:style>
+              <a:lnRef idx="0">
+                <a:scrgbClr r="0" g="0" b="0"/>
+              </a:lnRef>
+              <a:fillRef idx="0">
+                <a:scrgbClr r="0" g="0" b="0"/>
+              </a:fillRef>
+              <a:effectRef idx="0">
+                <a:scrgbClr r="0" g="0" b="0"/>
+              </a:effectRef>
+              <a:fontRef idx="minor">
+                <a:schemeClr val="tx1"/>
+              </a:fontRef>
+            </xdr:style>
+            <xdr:txBody>
+              <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+                <a:noAutofit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="2800" b="1">
+                    <a:solidFill>
+                      <a:srgbClr val="FF0000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Centaur" panose="02030504050205020304" pitchFamily="18" charset="0"/>
+                  </a:rPr>
+                  <a:t>3)</a:t>
+                </a:r>
+                <a:endParaRPr lang="cs-CZ" sz="2800" b="1">
+                  <a:solidFill>
+                    <a:srgbClr val="FF0000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Centaur" panose="02030504050205020304" pitchFamily="18" charset="0"/>
+                </a:endParaRPr>
+              </a:p>
+            </xdr:txBody>
+          </xdr:sp>
+        </xdr:grpSp>
+        <xdr:grpSp>
+          <xdr:nvGrpSpPr>
+            <xdr:cNvPr id="101" name="Skupina 100"/>
+            <xdr:cNvGrpSpPr/>
+          </xdr:nvGrpSpPr>
+          <xdr:grpSpPr>
+            <a:xfrm>
+              <a:off x="13044767" y="22791964"/>
+              <a:ext cx="5010737" cy="2590800"/>
+              <a:chOff x="14149667" y="22593300"/>
+              <a:chExt cx="4984883" cy="2590800"/>
+            </a:xfrm>
+          </xdr:grpSpPr>
+          <xdr:pic>
+            <xdr:nvPicPr>
+              <xdr:cNvPr id="99" name="Obrázek 98"/>
+              <xdr:cNvPicPr>
+                <a:picLocks noChangeAspect="1"/>
+              </xdr:cNvPicPr>
+            </xdr:nvPicPr>
+            <xdr:blipFill>
+              <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId22"/>
+              <a:stretch>
+                <a:fillRect/>
+              </a:stretch>
+            </xdr:blipFill>
+            <xdr:spPr>
+              <a:xfrm>
+                <a:off x="14544675" y="22593300"/>
+                <a:ext cx="4589875" cy="2590800"/>
+              </a:xfrm>
+              <a:prstGeom prst="rect">
+                <a:avLst/>
+              </a:prstGeom>
+            </xdr:spPr>
+          </xdr:pic>
+          <xdr:sp macro="" textlink="">
+            <xdr:nvSpPr>
+              <xdr:cNvPr id="100" name="TextovéPole 99"/>
+              <xdr:cNvSpPr txBox="1"/>
+            </xdr:nvSpPr>
+            <xdr:spPr>
+              <a:xfrm>
+                <a:off x="14149667" y="23237076"/>
+                <a:ext cx="785524" cy="501676"/>
+              </a:xfrm>
+              <a:prstGeom prst="rect">
+                <a:avLst/>
+              </a:prstGeom>
+              <a:noFill/>
+            </xdr:spPr>
+            <xdr:style>
+              <a:lnRef idx="0">
+                <a:scrgbClr r="0" g="0" b="0"/>
+              </a:lnRef>
+              <a:fillRef idx="0">
+                <a:scrgbClr r="0" g="0" b="0"/>
+              </a:fillRef>
+              <a:effectRef idx="0">
+                <a:scrgbClr r="0" g="0" b="0"/>
+              </a:effectRef>
+              <a:fontRef idx="minor">
+                <a:schemeClr val="tx1"/>
+              </a:fontRef>
+            </xdr:style>
+            <xdr:txBody>
+              <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+                <a:noAutofit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="2800" b="1">
+                    <a:solidFill>
+                      <a:srgbClr val="FF0000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Centaur" panose="02030504050205020304" pitchFamily="18" charset="0"/>
+                  </a:rPr>
+                  <a:t>2)</a:t>
+                </a:r>
+                <a:endParaRPr lang="cs-CZ" sz="2800" b="1">
+                  <a:solidFill>
+                    <a:srgbClr val="FF0000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Centaur" panose="02030504050205020304" pitchFamily="18" charset="0"/>
+                </a:endParaRPr>
+              </a:p>
+            </xdr:txBody>
+          </xdr:sp>
+        </xdr:grpSp>
+        <xdr:grpSp>
+          <xdr:nvGrpSpPr>
+            <xdr:cNvPr id="106" name="Skupina 105"/>
+            <xdr:cNvGrpSpPr/>
+          </xdr:nvGrpSpPr>
+          <xdr:grpSpPr>
+            <a:xfrm>
+              <a:off x="13362215" y="28194000"/>
+              <a:ext cx="4818821" cy="2588091"/>
+              <a:chOff x="13158107" y="28194000"/>
+              <a:chExt cx="4818821" cy="2588091"/>
+            </a:xfrm>
+          </xdr:grpSpPr>
+          <xdr:pic>
+            <xdr:nvPicPr>
+              <xdr:cNvPr id="104" name="Obrázek 103"/>
+              <xdr:cNvPicPr>
+                <a:picLocks noChangeAspect="1"/>
+              </xdr:cNvPicPr>
+            </xdr:nvPicPr>
+            <xdr:blipFill>
+              <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId23"/>
+              <a:stretch>
+                <a:fillRect/>
+              </a:stretch>
+            </xdr:blipFill>
+            <xdr:spPr>
+              <a:xfrm>
+                <a:off x="13158107" y="28194000"/>
+                <a:ext cx="4818821" cy="2540959"/>
+              </a:xfrm>
+              <a:prstGeom prst="rect">
+                <a:avLst/>
+              </a:prstGeom>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+            </xdr:spPr>
+          </xdr:pic>
+          <xdr:sp macro="" textlink="">
+            <xdr:nvSpPr>
+              <xdr:cNvPr id="105" name="TextovéPole 104"/>
+              <xdr:cNvSpPr txBox="1"/>
+            </xdr:nvSpPr>
+            <xdr:spPr>
+              <a:xfrm>
+                <a:off x="13628352" y="30280415"/>
+                <a:ext cx="790664" cy="501676"/>
+              </a:xfrm>
+              <a:prstGeom prst="rect">
+                <a:avLst/>
+              </a:prstGeom>
+              <a:noFill/>
+            </xdr:spPr>
+            <xdr:style>
+              <a:lnRef idx="0">
+                <a:scrgbClr r="0" g="0" b="0"/>
+              </a:lnRef>
+              <a:fillRef idx="0">
+                <a:scrgbClr r="0" g="0" b="0"/>
+              </a:fillRef>
+              <a:effectRef idx="0">
+                <a:scrgbClr r="0" g="0" b="0"/>
+              </a:effectRef>
+              <a:fontRef idx="minor">
+                <a:schemeClr val="tx1"/>
+              </a:fontRef>
+            </xdr:style>
+            <xdr:txBody>
+              <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+                <a:noAutofit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="2800" b="1">
+                    <a:solidFill>
+                      <a:srgbClr val="FF0000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Centaur" panose="02030504050205020304" pitchFamily="18" charset="0"/>
+                  </a:rPr>
+                  <a:t>4)</a:t>
+                </a:r>
+                <a:endParaRPr lang="cs-CZ" sz="2800" b="1">
+                  <a:solidFill>
+                    <a:srgbClr val="FF0000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Centaur" panose="02030504050205020304" pitchFamily="18" charset="0"/>
+                </a:endParaRPr>
+              </a:p>
+            </xdr:txBody>
+          </xdr:sp>
+        </xdr:grpSp>
+      </xdr:grpSp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="36" name="Obdélník 35"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="32368671" y="12676414"/>
+            <a:ext cx="13778593" cy="10591800"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln w="28575">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="cs-CZ" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>81644</xdr:colOff>
+      <xdr:row>148</xdr:row>
+      <xdr:rowOff>81643</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>408215</xdr:colOff>
+      <xdr:row>169</xdr:row>
+      <xdr:rowOff>108857</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="55" name="Skupina 54"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="7396844" y="28428043"/>
+          <a:ext cx="3984171" cy="4027714"/>
+          <a:chOff x="7320643" y="28370893"/>
+          <a:chExt cx="4000500" cy="4027714"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:grpSp>
+        <xdr:nvGrpSpPr>
+          <xdr:cNvPr id="98" name="Skupina 97"/>
+          <xdr:cNvGrpSpPr/>
+        </xdr:nvGrpSpPr>
+        <xdr:grpSpPr>
+          <a:xfrm>
+            <a:off x="7533111" y="28622624"/>
+            <a:ext cx="3536198" cy="3552118"/>
+            <a:chOff x="13139248" y="27241500"/>
+            <a:chExt cx="3519633" cy="3552118"/>
+          </a:xfrm>
+        </xdr:grpSpPr>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="61" name="Obrázek 60"/>
+            <xdr:cNvPicPr>
+              <a:picLocks noChangeAspect="1"/>
+            </xdr:cNvPicPr>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId24"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="13189324" y="29622189"/>
+              <a:ext cx="3464989" cy="1171429"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:pic>
+        <xdr:grpSp>
+          <xdr:nvGrpSpPr>
+            <xdr:cNvPr id="97" name="Skupina 96"/>
+            <xdr:cNvGrpSpPr/>
+          </xdr:nvGrpSpPr>
+          <xdr:grpSpPr>
+            <a:xfrm>
+              <a:off x="13139248" y="27241500"/>
+              <a:ext cx="3519633" cy="2285714"/>
+              <a:chOff x="13139248" y="27241500"/>
+              <a:chExt cx="3519633" cy="2285714"/>
+            </a:xfrm>
+          </xdr:grpSpPr>
+          <xdr:sp macro="" textlink="">
+            <xdr:nvSpPr>
+              <xdr:cNvPr id="16" name="TextovéPole 15"/>
+              <xdr:cNvSpPr txBox="1"/>
+            </xdr:nvSpPr>
+            <xdr:spPr>
+              <a:xfrm>
+                <a:off x="13139248" y="27439841"/>
+                <a:ext cx="777006" cy="501676"/>
+              </a:xfrm>
+              <a:prstGeom prst="rect">
+                <a:avLst/>
+              </a:prstGeom>
+              <a:noFill/>
+            </xdr:spPr>
+            <xdr:style>
+              <a:lnRef idx="0">
+                <a:scrgbClr r="0" g="0" b="0"/>
+              </a:lnRef>
+              <a:fillRef idx="0">
+                <a:scrgbClr r="0" g="0" b="0"/>
+              </a:fillRef>
+              <a:effectRef idx="0">
+                <a:scrgbClr r="0" g="0" b="0"/>
+              </a:effectRef>
+              <a:fontRef idx="minor">
+                <a:schemeClr val="tx1"/>
+              </a:fontRef>
+            </xdr:style>
+            <xdr:txBody>
+              <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="2800" b="1">
+                    <a:solidFill>
+                      <a:srgbClr val="FF0000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Centaur" panose="02030504050205020304" pitchFamily="18" charset="0"/>
+                  </a:rPr>
+                  <a:t>VIII</a:t>
+                </a:r>
+                <a:endParaRPr lang="cs-CZ" sz="2800" b="1">
+                  <a:solidFill>
+                    <a:srgbClr val="FF0000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Centaur" panose="02030504050205020304" pitchFamily="18" charset="0"/>
+                </a:endParaRPr>
+              </a:p>
+            </xdr:txBody>
+          </xdr:sp>
+          <xdr:grpSp>
+            <xdr:nvGrpSpPr>
+              <xdr:cNvPr id="96" name="Skupina 95"/>
+              <xdr:cNvGrpSpPr/>
+            </xdr:nvGrpSpPr>
+            <xdr:grpSpPr>
+              <a:xfrm>
+                <a:off x="13906500" y="27241500"/>
+                <a:ext cx="2752381" cy="2285714"/>
+                <a:chOff x="13982700" y="28174950"/>
+                <a:chExt cx="2752381" cy="2285714"/>
+              </a:xfrm>
+            </xdr:grpSpPr>
+            <xdr:pic>
+              <xdr:nvPicPr>
+                <xdr:cNvPr id="93" name="Obrázek 92"/>
+                <xdr:cNvPicPr>
+                  <a:picLocks noChangeAspect="1"/>
+                </xdr:cNvPicPr>
+              </xdr:nvPicPr>
+              <xdr:blipFill>
+                <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId25"/>
+                <a:stretch>
+                  <a:fillRect/>
+                </a:stretch>
+              </xdr:blipFill>
+              <xdr:spPr>
+                <a:xfrm>
+                  <a:off x="13982700" y="28174950"/>
+                  <a:ext cx="2752381" cy="2285714"/>
+                </a:xfrm>
+                <a:prstGeom prst="rect">
+                  <a:avLst/>
+                </a:prstGeom>
+                <a:ln>
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                </a:ln>
+              </xdr:spPr>
+            </xdr:pic>
+            <xdr:sp macro="" textlink="">
+              <xdr:nvSpPr>
+                <xdr:cNvPr id="94" name="Obdélník 93"/>
+                <xdr:cNvSpPr/>
+              </xdr:nvSpPr>
+              <xdr:spPr>
+                <a:xfrm>
+                  <a:off x="16149917" y="28987497"/>
+                  <a:ext cx="334266" cy="267009"/>
+                </a:xfrm>
+                <a:prstGeom prst="rect">
+                  <a:avLst/>
+                </a:prstGeom>
+                <a:noFill/>
+                <a:ln w="38100">
+                  <a:solidFill>
+                    <a:srgbClr val="FF0000"/>
+                  </a:solidFill>
+                </a:ln>
+              </xdr:spPr>
+              <xdr:style>
+                <a:lnRef idx="2">
+                  <a:schemeClr val="accent1">
+                    <a:shade val="50000"/>
+                  </a:schemeClr>
+                </a:lnRef>
+                <a:fillRef idx="1">
+                  <a:schemeClr val="accent1"/>
+                </a:fillRef>
+                <a:effectRef idx="0">
+                  <a:schemeClr val="accent1"/>
+                </a:effectRef>
+                <a:fontRef idx="minor">
+                  <a:schemeClr val="lt1"/>
+                </a:fontRef>
+              </xdr:style>
+              <xdr:txBody>
+                <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr algn="l"/>
+                  <a:endParaRPr lang="cs-CZ" sz="1100"/>
+                </a:p>
+              </xdr:txBody>
+            </xdr:sp>
+            <xdr:sp macro="" textlink="">
+              <xdr:nvSpPr>
+                <xdr:cNvPr id="95" name="Obdélník 94"/>
+                <xdr:cNvSpPr/>
+              </xdr:nvSpPr>
+              <xdr:spPr>
+                <a:xfrm>
+                  <a:off x="15582900" y="28336875"/>
+                  <a:ext cx="504825" cy="904875"/>
+                </a:xfrm>
+                <a:prstGeom prst="rect">
+                  <a:avLst/>
+                </a:prstGeom>
+                <a:noFill/>
+                <a:ln w="38100">
+                  <a:solidFill>
+                    <a:srgbClr val="FF0000"/>
+                  </a:solidFill>
+                </a:ln>
+              </xdr:spPr>
+              <xdr:style>
+                <a:lnRef idx="2">
+                  <a:schemeClr val="accent1">
+                    <a:shade val="50000"/>
+                  </a:schemeClr>
+                </a:lnRef>
+                <a:fillRef idx="1">
+                  <a:schemeClr val="accent1"/>
+                </a:fillRef>
+                <a:effectRef idx="0">
+                  <a:schemeClr val="accent1"/>
+                </a:effectRef>
+                <a:fontRef idx="minor">
+                  <a:schemeClr val="lt1"/>
+                </a:fontRef>
+              </xdr:style>
+              <xdr:txBody>
+                <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr algn="l"/>
+                  <a:endParaRPr lang="cs-CZ" sz="1100"/>
+                </a:p>
+              </xdr:txBody>
+            </xdr:sp>
+          </xdr:grpSp>
+        </xdr:grpSp>
+      </xdr:grpSp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="46" name="Obdélník 45"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="7320643" y="28370893"/>
+            <a:ext cx="4000500" cy="4027714"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln w="28575">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="cs-CZ" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>68035</xdr:colOff>
+      <xdr:row>170</xdr:row>
+      <xdr:rowOff>108857</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>233</xdr:row>
+      <xdr:rowOff>11189</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="79" name="Skupina 78"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="7383235" y="32646257"/>
+          <a:ext cx="6723290" cy="11903832"/>
+          <a:chOff x="7383235" y="32646257"/>
+          <a:chExt cx="6723290" cy="11903832"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:grpSp>
+        <xdr:nvGrpSpPr>
+          <xdr:cNvPr id="78" name="Skupina 77"/>
+          <xdr:cNvGrpSpPr/>
+        </xdr:nvGrpSpPr>
+        <xdr:grpSpPr>
+          <a:xfrm>
+            <a:off x="7383235" y="32646257"/>
+            <a:ext cx="6452788" cy="11903832"/>
+            <a:chOff x="7464878" y="32795936"/>
+            <a:chExt cx="6452788" cy="11903832"/>
+          </a:xfrm>
+        </xdr:grpSpPr>
+        <xdr:grpSp>
+          <xdr:nvGrpSpPr>
+            <xdr:cNvPr id="75" name="Skupina 74"/>
+            <xdr:cNvGrpSpPr/>
+          </xdr:nvGrpSpPr>
+          <xdr:grpSpPr>
+            <a:xfrm>
+              <a:off x="7464878" y="32795936"/>
+              <a:ext cx="6452786" cy="4314286"/>
+              <a:chOff x="7443107" y="34140321"/>
+              <a:chExt cx="6714286" cy="4314286"/>
+            </a:xfrm>
+          </xdr:grpSpPr>
+          <xdr:pic>
+            <xdr:nvPicPr>
+              <xdr:cNvPr id="70" name="Obrázek 69"/>
+              <xdr:cNvPicPr>
+                <a:picLocks noChangeAspect="1"/>
+              </xdr:cNvPicPr>
+            </xdr:nvPicPr>
+            <xdr:blipFill>
+              <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId26"/>
+              <a:stretch>
+                <a:fillRect/>
+              </a:stretch>
+            </xdr:blipFill>
+            <xdr:spPr>
+              <a:xfrm>
+                <a:off x="7443107" y="34140321"/>
+                <a:ext cx="6714286" cy="4314286"/>
+              </a:xfrm>
+              <a:prstGeom prst="rect">
+                <a:avLst/>
+              </a:prstGeom>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+            </xdr:spPr>
+          </xdr:pic>
+          <xdr:sp macro="" textlink="">
+            <xdr:nvSpPr>
+              <xdr:cNvPr id="102" name="TextovéPole 101"/>
+              <xdr:cNvSpPr txBox="1"/>
+            </xdr:nvSpPr>
+            <xdr:spPr>
+              <a:xfrm>
+                <a:off x="10382251" y="34181142"/>
+                <a:ext cx="780663" cy="501676"/>
+              </a:xfrm>
+              <a:prstGeom prst="rect">
+                <a:avLst/>
+              </a:prstGeom>
+              <a:noFill/>
+            </xdr:spPr>
+            <xdr:style>
+              <a:lnRef idx="0">
+                <a:scrgbClr r="0" g="0" b="0"/>
+              </a:lnRef>
+              <a:fillRef idx="0">
+                <a:scrgbClr r="0" g="0" b="0"/>
+              </a:fillRef>
+              <a:effectRef idx="0">
+                <a:scrgbClr r="0" g="0" b="0"/>
+              </a:effectRef>
+              <a:fontRef idx="minor">
+                <a:schemeClr val="tx1"/>
+              </a:fontRef>
+            </xdr:style>
+            <xdr:txBody>
+              <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+                <a:noAutofit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="2800" b="1">
+                    <a:solidFill>
+                      <a:srgbClr val="FF0000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Centaur" panose="02030504050205020304" pitchFamily="18" charset="0"/>
+                  </a:rPr>
+                  <a:t>IX</a:t>
+                </a:r>
+                <a:endParaRPr lang="cs-CZ" sz="2800" b="1">
+                  <a:solidFill>
+                    <a:srgbClr val="FF0000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Centaur" panose="02030504050205020304" pitchFamily="18" charset="0"/>
+                </a:endParaRPr>
+              </a:p>
+            </xdr:txBody>
+          </xdr:sp>
+        </xdr:grpSp>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="76" name="Obrázek 75"/>
+            <xdr:cNvPicPr>
+              <a:picLocks noChangeAspect="1"/>
+            </xdr:cNvPicPr>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId27"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="7464880" y="37150223"/>
+              <a:ext cx="6452786" cy="3651109"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:pic>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="77" name="Obrázek 76"/>
+            <xdr:cNvPicPr>
+              <a:picLocks noChangeAspect="1"/>
+            </xdr:cNvPicPr>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId28"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="7464879" y="40810543"/>
+              <a:ext cx="6452786" cy="3889225"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:pic>
+      </xdr:grpSp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="108" name="TextovéPole 107"/>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="9250135" y="39256606"/>
+            <a:ext cx="4856390" cy="1281793"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+            <a:noAutofit/>
+          </a:bodyPr>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-GB" sz="2800" b="1">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+                <a:latin typeface="Centaur" panose="02030504050205020304" pitchFamily="18" charset="0"/>
+              </a:rPr>
+              <a:t>This</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" sz="2800" b="1" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+                <a:latin typeface="Centaur" panose="02030504050205020304" pitchFamily="18" charset="0"/>
+              </a:rPr>
+              <a:t> is not gonna be applied.</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-GB" sz="2800" b="1" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+                <a:latin typeface="Centaur" panose="02030504050205020304" pitchFamily="18" charset="0"/>
+              </a:rPr>
+              <a:t>Requires biaxial tensile failure test.</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:endParaRPr lang="en-GB" sz="2800" b="1" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:latin typeface="Centaur" panose="02030504050205020304" pitchFamily="18" charset="0"/>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -3996,8 +4406,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="14341296" y="138367"/>
-          <a:ext cx="5079244" cy="4638612"/>
+          <a:off x="14317976" y="138367"/>
+          <a:ext cx="5068734" cy="4648465"/>
           <a:chOff x="6626087" y="4265543"/>
           <a:chExt cx="5095238" cy="4634092"/>
         </a:xfrm>
@@ -4081,8 +4491,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="10074643" y="238126"/>
-          <a:ext cx="4231896" cy="4475120"/>
+          <a:off x="10060520" y="238126"/>
+          <a:ext cx="4222699" cy="4484973"/>
           <a:chOff x="10003930" y="238126"/>
           <a:chExt cx="4191323" cy="4479370"/>
         </a:xfrm>
@@ -4476,17 +4886,64 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A45:A62"/>
+  <dimension ref="A2:AQ62"/>
   <sheetViews>
-    <sheetView topLeftCell="B8" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J37" sqref="J37"/>
+    <sheetView tabSelected="1" topLeftCell="J161" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K168" sqref="K168"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="29" max="29" width="10.7109375" customWidth="1"/>
+    <col min="38" max="38" width="9.140625" style="66"/>
   </cols>
   <sheetData>
+    <row r="2" spans="39:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="39:43" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AM3" s="67" t="s">
+        <v>59</v>
+      </c>
+      <c r="AN3" s="67"/>
+      <c r="AO3" s="67"/>
+      <c r="AP3" s="67"/>
+      <c r="AQ3" s="67"/>
+    </row>
+    <row r="4" spans="39:43" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AM4" s="67"/>
+      <c r="AN4" s="67"/>
+      <c r="AO4" s="67"/>
+      <c r="AP4" s="67"/>
+      <c r="AQ4" s="67"/>
+    </row>
+    <row r="5" spans="39:43" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AM5" s="67"/>
+      <c r="AN5" s="67"/>
+      <c r="AO5" s="67"/>
+      <c r="AP5" s="67"/>
+      <c r="AQ5" s="67"/>
+    </row>
+    <row r="6" spans="39:43" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AM6" s="67"/>
+      <c r="AN6" s="67"/>
+      <c r="AO6" s="67"/>
+      <c r="AP6" s="67"/>
+      <c r="AQ6" s="67"/>
+    </row>
+    <row r="7" spans="39:43" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AM7" s="67"/>
+      <c r="AN7" s="67"/>
+      <c r="AO7" s="67"/>
+      <c r="AP7" s="67"/>
+      <c r="AQ7" s="67"/>
+    </row>
+    <row r="8" spans="39:43" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AM8" s="67"/>
+      <c r="AN8" s="67"/>
+      <c r="AO8" s="67"/>
+      <c r="AP8" s="67"/>
+      <c r="AQ8" s="67"/>
+    </row>
+    <row r="9" spans="39:43" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="45" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>0</v>
@@ -4548,8 +5005,12 @@
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="AM3:AQ8"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -4560,8 +5021,8 @@
   </sheetPr>
   <dimension ref="A1:M22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4570,14 +5031,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="39.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="66" t="s">
-        <v>44</v>
-      </c>
-      <c r="B1" s="67"/>
-      <c r="C1" s="67"/>
-      <c r="D1" s="67"/>
-      <c r="E1" s="67"/>
-      <c r="F1" s="67"/>
+      <c r="A1" s="68" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="69"/>
+      <c r="C1" s="69"/>
+      <c r="D1" s="69"/>
+      <c r="E1" s="69"/>
+      <c r="F1" s="69"/>
     </row>
     <row r="2" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -4621,59 +5082,59 @@
       <c r="A4" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="68" t="s">
-        <v>50</v>
-      </c>
-      <c r="C4" s="69"/>
+      <c r="B4" s="70" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4" s="71"/>
       <c r="D4" s="36" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E4" s="37" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="F4" s="38" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G4" s="39" t="s">
         <v>48</v>
       </c>
       <c r="H4" s="40" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="I4" s="41" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="J4" s="42" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="K4" s="43" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="L4" s="44" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="M4" s="45" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="47" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B5" s="48" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" s="61" t="s">
+        <v>50</v>
+      </c>
+      <c r="D5" s="51">
+        <v>0</v>
+      </c>
+      <c r="E5" s="52">
         <v>45</v>
       </c>
-      <c r="C5" s="61" t="s">
-        <v>51</v>
-      </c>
-      <c r="D5" s="51">
-        <v>90</v>
-      </c>
-      <c r="E5" s="52">
-        <v>0</v>
-      </c>
       <c r="F5" s="53">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="G5" s="54">
         <v>45</v>
@@ -4721,19 +5182,19 @@
       </c>
       <c r="G6" s="5">
         <f>HLOOKUP(G$4,Material_Database!$D$4:$N$16,2,0)</f>
-        <v>57450</v>
+        <v>0</v>
       </c>
       <c r="H6" s="5">
         <f>HLOOKUP(H$4,Material_Database!$D$4:$N$16,2,0)</f>
-        <v>57450</v>
+        <v>0</v>
       </c>
       <c r="I6" s="5">
         <f>HLOOKUP(I$4,Material_Database!$D$4:$N$16,2,0)</f>
-        <v>57450</v>
+        <v>0</v>
       </c>
       <c r="J6" s="5">
         <f>HLOOKUP(J$4,Material_Database!$D$4:$N$16,2,0)</f>
-        <v>57450</v>
+        <v>0</v>
       </c>
       <c r="K6" s="5">
         <f>HLOOKUP(K$4,Material_Database!$D$4:$N$16,2,0)</f>
@@ -4772,19 +5233,19 @@
       </c>
       <c r="G7" s="5">
         <f>HLOOKUP(G$4,Material_Database!$D$4:$N$16,3,0)</f>
-        <v>57450</v>
+        <v>0</v>
       </c>
       <c r="H7" s="5">
         <f>HLOOKUP(H$4,Material_Database!$D$4:$N$16,3,0)</f>
-        <v>57450</v>
+        <v>0</v>
       </c>
       <c r="I7" s="5">
         <f>HLOOKUP(I$4,Material_Database!$D$4:$N$16,3,0)</f>
-        <v>57450</v>
+        <v>0</v>
       </c>
       <c r="J7" s="5">
         <f>HLOOKUP(J$4,Material_Database!$D$4:$N$16,3,0)</f>
-        <v>57450</v>
+        <v>0</v>
       </c>
       <c r="K7" s="5">
         <f>HLOOKUP(K$4,Material_Database!$D$4:$N$16,3,0)</f>
@@ -4823,19 +5284,19 @@
       </c>
       <c r="G8" s="5">
         <f>HLOOKUP(G$4,Material_Database!$D$4:$N$16,4,0)</f>
-        <v>2630</v>
+        <v>0</v>
       </c>
       <c r="H8" s="5">
         <f>HLOOKUP(H$4,Material_Database!$D$4:$N$16,4,0)</f>
-        <v>2630</v>
+        <v>0</v>
       </c>
       <c r="I8" s="5">
         <f>HLOOKUP(I$4,Material_Database!$D$4:$N$16,4,0)</f>
-        <v>2630</v>
+        <v>0</v>
       </c>
       <c r="J8" s="5">
         <f>HLOOKUP(J$4,Material_Database!$D$4:$N$16,4,0)</f>
-        <v>2630</v>
+        <v>0</v>
       </c>
       <c r="K8" s="5">
         <f>HLOOKUP(K$4,Material_Database!$D$4:$N$16,4,0)</f>
@@ -4874,19 +5335,19 @@
       </c>
       <c r="G9" s="5">
         <f>HLOOKUP(G$4,Material_Database!$D$4:$N$16,5,0)</f>
-        <v>3.6999999999999998E-2</v>
+        <v>0</v>
       </c>
       <c r="H9" s="5">
         <f>HLOOKUP(H$4,Material_Database!$D$4:$N$16,5,0)</f>
-        <v>3.6999999999999998E-2</v>
+        <v>0</v>
       </c>
       <c r="I9" s="5">
         <f>HLOOKUP(I$4,Material_Database!$D$4:$N$16,5,0)</f>
-        <v>3.6999999999999998E-2</v>
+        <v>0</v>
       </c>
       <c r="J9" s="5">
         <f>HLOOKUP(J$4,Material_Database!$D$4:$N$16,5,0)</f>
-        <v>3.6999999999999998E-2</v>
+        <v>0</v>
       </c>
       <c r="K9" s="5">
         <f>HLOOKUP(K$4,Material_Database!$D$4:$N$16,5,0)</f>
@@ -4925,19 +5386,19 @@
       </c>
       <c r="G10" s="5">
         <f>HLOOKUP(G$4,Material_Database!$D$4:$N$16,6,0)</f>
-        <v>700</v>
+        <v>0</v>
       </c>
       <c r="H10" s="5">
         <f>HLOOKUP(H$4,Material_Database!$D$4:$N$16,6,0)</f>
-        <v>700</v>
+        <v>0</v>
       </c>
       <c r="I10" s="5">
         <f>HLOOKUP(I$4,Material_Database!$D$4:$N$16,6,0)</f>
-        <v>700</v>
+        <v>0</v>
       </c>
       <c r="J10" s="5">
         <f>HLOOKUP(J$4,Material_Database!$D$4:$N$16,6,0)</f>
-        <v>700</v>
+        <v>0</v>
       </c>
       <c r="K10" s="5">
         <f>HLOOKUP(K$4,Material_Database!$D$4:$N$16,6,0)</f>
@@ -4957,7 +5418,7 @@
         <v>23</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C11" s="62" t="s">
         <v>31</v>
@@ -4976,19 +5437,19 @@
       </c>
       <c r="G11" s="5">
         <f>HLOOKUP(G$4,Material_Database!$D$4:$N$16,7,0)</f>
-        <v>350</v>
+        <v>0</v>
       </c>
       <c r="H11" s="5">
         <f>HLOOKUP(H$4,Material_Database!$D$4:$N$16,7,0)</f>
-        <v>350</v>
+        <v>0</v>
       </c>
       <c r="I11" s="5">
         <f>HLOOKUP(I$4,Material_Database!$D$4:$N$16,7,0)</f>
-        <v>350</v>
+        <v>0</v>
       </c>
       <c r="J11" s="5">
         <f>HLOOKUP(J$4,Material_Database!$D$4:$N$16,7,0)</f>
-        <v>350</v>
+        <v>0</v>
       </c>
       <c r="K11" s="5">
         <f>HLOOKUP(K$4,Material_Database!$D$4:$N$16,7,0)</f>
@@ -5027,19 +5488,19 @@
       </c>
       <c r="G12" s="5">
         <f>HLOOKUP(G$4,Material_Database!$D$4:$N$16,8,0)</f>
-        <v>700</v>
+        <v>0</v>
       </c>
       <c r="H12" s="5">
         <f>HLOOKUP(H$4,Material_Database!$D$4:$N$16,8,0)</f>
-        <v>700</v>
+        <v>0</v>
       </c>
       <c r="I12" s="5">
         <f>HLOOKUP(I$4,Material_Database!$D$4:$N$16,8,0)</f>
-        <v>700</v>
+        <v>0</v>
       </c>
       <c r="J12" s="5">
         <f>HLOOKUP(J$4,Material_Database!$D$4:$N$16,8,0)</f>
-        <v>700</v>
+        <v>0</v>
       </c>
       <c r="K12" s="5">
         <f>HLOOKUP(K$4,Material_Database!$D$4:$N$16,8,0)</f>
@@ -5059,7 +5520,7 @@
         <v>25</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C13" s="62" t="s">
         <v>31</v>
@@ -5078,19 +5539,19 @@
       </c>
       <c r="G13" s="5">
         <f>HLOOKUP(G$4,Material_Database!$D$4:$N$16,9,0)</f>
-        <v>350</v>
+        <v>0</v>
       </c>
       <c r="H13" s="5">
         <f>HLOOKUP(H$4,Material_Database!$D$4:$N$16,9,0)</f>
-        <v>350</v>
+        <v>0</v>
       </c>
       <c r="I13" s="5">
         <f>HLOOKUP(I$4,Material_Database!$D$4:$N$16,9,0)</f>
-        <v>350</v>
+        <v>0</v>
       </c>
       <c r="J13" s="5">
         <f>HLOOKUP(J$4,Material_Database!$D$4:$N$16,9,0)</f>
-        <v>350</v>
+        <v>0</v>
       </c>
       <c r="K13" s="5">
         <f>HLOOKUP(K$4,Material_Database!$D$4:$N$16,9,0)</f>
@@ -5129,19 +5590,19 @@
       </c>
       <c r="G14" s="5">
         <f>HLOOKUP(G$4,Material_Database!$D$4:$N$16,10,0)</f>
-        <v>70</v>
+        <v>0</v>
       </c>
       <c r="H14" s="5">
         <f>HLOOKUP(H$4,Material_Database!$D$4:$N$16,10,0)</f>
-        <v>70</v>
+        <v>0</v>
       </c>
       <c r="I14" s="5">
         <f>HLOOKUP(I$4,Material_Database!$D$4:$N$16,10,0)</f>
-        <v>70</v>
+        <v>0</v>
       </c>
       <c r="J14" s="5">
         <f>HLOOKUP(J$4,Material_Database!$D$4:$N$16,10,0)</f>
-        <v>70</v>
+        <v>0</v>
       </c>
       <c r="K14" s="5">
         <f>HLOOKUP(K$4,Material_Database!$D$4:$N$16,10,0)</f>
@@ -5172,7 +5633,7 @@
       </c>
       <c r="E15" s="5">
         <f>HLOOKUP(E$4,Material_Database!$D$4:$N$16,11,0)</f>
-        <v>0.5</v>
+        <v>0.22</v>
       </c>
       <c r="F15" s="5">
         <f>HLOOKUP(F$4,Material_Database!$D$4:$N$16,11,0)</f>
@@ -5180,19 +5641,19 @@
       </c>
       <c r="G15" s="5">
         <f>HLOOKUP(G$4,Material_Database!$D$4:$N$16,11,0)</f>
-        <v>0.22</v>
+        <v>0</v>
       </c>
       <c r="H15" s="5">
         <f>HLOOKUP(H$4,Material_Database!$D$4:$N$16,11,0)</f>
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="I15" s="5">
         <f>HLOOKUP(I$4,Material_Database!$D$4:$N$16,11,0)</f>
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="J15" s="5">
         <f>HLOOKUP(J$4,Material_Database!$D$4:$N$16,11,0)</f>
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="K15" s="5">
         <f>HLOOKUP(K$4,Material_Database!$D$4:$N$16,11,0)</f>
@@ -5231,19 +5692,19 @@
       </c>
       <c r="G16" s="5">
         <f>HLOOKUP(G$4,Material_Database!$D$4:$N$16,12,0)</f>
-        <v>1460</v>
+        <v>0</v>
       </c>
       <c r="H16" s="5">
         <f>HLOOKUP(H$4,Material_Database!$D$4:$N$16,12,0)</f>
-        <v>1460</v>
+        <v>0</v>
       </c>
       <c r="I16" s="5">
         <f>HLOOKUP(I$4,Material_Database!$D$4:$N$16,12,0)</f>
-        <v>1460</v>
+        <v>0</v>
       </c>
       <c r="J16" s="5">
         <f>HLOOKUP(J$4,Material_Database!$D$4:$N$16,12,0)</f>
-        <v>1460</v>
+        <v>0</v>
       </c>
       <c r="K16" s="5">
         <f>HLOOKUP(K$4,Material_Database!$D$4:$N$16,12,0)</f>
@@ -5282,19 +5743,19 @@
       </c>
       <c r="G17" s="49">
         <f>HLOOKUP(G$4,Material_Database!$D$4:$N$16,13,0)</f>
-        <v>321.2</v>
+        <v>0</v>
       </c>
       <c r="H17" s="49">
         <f>HLOOKUP(H$4,Material_Database!$D$4:$N$16,13,0)</f>
-        <v>321.2</v>
+        <v>0</v>
       </c>
       <c r="I17" s="49">
         <f>HLOOKUP(I$4,Material_Database!$D$4:$N$16,13,0)</f>
-        <v>321.2</v>
+        <v>0</v>
       </c>
       <c r="J17" s="49">
         <f>HLOOKUP(J$4,Material_Database!$D$4:$N$16,13,0)</f>
-        <v>321.2</v>
+        <v>0</v>
       </c>
       <c r="K17" s="49">
         <f>HLOOKUP(K$4,Material_Database!$D$4:$N$16,13,0)</f>
@@ -5314,11 +5775,11 @@
     </row>
     <row r="20" spans="1:13" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C20" s="2">
         <f>SUM(D17:M17)</f>
-        <v>2248.4</v>
+        <v>963.59999999999991</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>35</v>
@@ -5330,11 +5791,11 @@
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C22" s="2">
         <f>SUM(D15:M15)</f>
-        <v>2.66</v>
+        <v>0.66</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>33</v>
@@ -5369,10 +5830,10 @@
   <sheetPr>
     <tabColor rgb="FF3399FF"/>
   </sheetPr>
-  <dimension ref="A1:N16"/>
+  <dimension ref="A1:N36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5383,13 +5844,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="31.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="70" t="s">
-        <v>43</v>
-      </c>
-      <c r="B1" s="67"/>
-      <c r="C1" s="67"/>
-      <c r="D1" s="67"/>
-      <c r="E1" s="67"/>
+      <c r="A1" s="72" t="s">
+        <v>57</v>
+      </c>
+      <c r="B1" s="69"/>
+      <c r="C1" s="69"/>
+      <c r="D1" s="69"/>
+      <c r="E1" s="69"/>
     </row>
     <row r="2" spans="1:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -5400,37 +5861,37 @@
       <c r="B4" s="20"/>
       <c r="C4" s="21"/>
       <c r="D4" s="64" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E4" s="22" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F4" s="20" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G4" s="20" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H4" s="20" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I4" s="20" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J4" s="20" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K4" s="20" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L4" s="20" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="M4" s="20" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="N4" s="21" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -5961,9 +6422,590 @@
         <v>0</v>
       </c>
     </row>
+    <row r="20" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="21" spans="1:14" ht="22.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="72" t="s">
+        <v>58</v>
+      </c>
+      <c r="B21" s="69"/>
+      <c r="C21" s="69"/>
+      <c r="D21" s="69"/>
+      <c r="E21" s="69"/>
+    </row>
+    <row r="22" spans="1:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="24" spans="1:14" ht="35.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="B24" s="20"/>
+      <c r="C24" s="21"/>
+      <c r="D24" s="64" t="s">
+        <v>48</v>
+      </c>
+      <c r="E24" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="F24" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="G24" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="H24" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="I24" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="J24" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="K24" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="L24" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="M24" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="N24" s="21" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C25" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="D25" s="7">
+        <v>0</v>
+      </c>
+      <c r="E25" s="15">
+        <v>0</v>
+      </c>
+      <c r="F25" s="15">
+        <v>0</v>
+      </c>
+      <c r="G25" s="9">
+        <v>0</v>
+      </c>
+      <c r="H25" s="9">
+        <v>0</v>
+      </c>
+      <c r="I25" s="9">
+        <v>0</v>
+      </c>
+      <c r="J25" s="9">
+        <v>0</v>
+      </c>
+      <c r="K25" s="9">
+        <v>0</v>
+      </c>
+      <c r="L25" s="9">
+        <v>0</v>
+      </c>
+      <c r="M25" s="9">
+        <v>0</v>
+      </c>
+      <c r="N25" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A26" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B26" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C26" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="D26" s="65">
+        <v>0</v>
+      </c>
+      <c r="E26" s="16">
+        <v>0</v>
+      </c>
+      <c r="F26" s="16">
+        <v>0</v>
+      </c>
+      <c r="G26" s="9">
+        <v>0</v>
+      </c>
+      <c r="H26" s="11">
+        <v>0</v>
+      </c>
+      <c r="I26" s="11">
+        <v>0</v>
+      </c>
+      <c r="J26" s="11">
+        <v>0</v>
+      </c>
+      <c r="K26" s="11">
+        <v>0</v>
+      </c>
+      <c r="L26" s="11">
+        <v>0</v>
+      </c>
+      <c r="M26" s="11">
+        <v>0</v>
+      </c>
+      <c r="N26" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A27" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B27" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C27" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="D27" s="65">
+        <v>0</v>
+      </c>
+      <c r="E27" s="16">
+        <v>0</v>
+      </c>
+      <c r="F27" s="16">
+        <v>0</v>
+      </c>
+      <c r="G27" s="9">
+        <v>0</v>
+      </c>
+      <c r="H27" s="11">
+        <v>0</v>
+      </c>
+      <c r="I27" s="11">
+        <v>0</v>
+      </c>
+      <c r="J27" s="11">
+        <v>0</v>
+      </c>
+      <c r="K27" s="11">
+        <v>0</v>
+      </c>
+      <c r="L27" s="11">
+        <v>0</v>
+      </c>
+      <c r="M27" s="11">
+        <v>0</v>
+      </c>
+      <c r="N27" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A28" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B28" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C28" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="D28" s="65">
+        <v>0</v>
+      </c>
+      <c r="E28" s="16">
+        <v>0</v>
+      </c>
+      <c r="F28" s="16">
+        <v>0</v>
+      </c>
+      <c r="G28" s="9">
+        <v>0</v>
+      </c>
+      <c r="H28" s="11">
+        <v>0</v>
+      </c>
+      <c r="I28" s="11">
+        <v>0</v>
+      </c>
+      <c r="J28" s="11">
+        <v>0</v>
+      </c>
+      <c r="K28" s="11">
+        <v>0</v>
+      </c>
+      <c r="L28" s="11">
+        <v>0</v>
+      </c>
+      <c r="M28" s="11">
+        <v>0</v>
+      </c>
+      <c r="N28" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" ht="18" x14ac:dyDescent="0.25">
+      <c r="A29" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B29" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="C29" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="D29" s="65">
+        <v>0</v>
+      </c>
+      <c r="E29" s="16">
+        <v>0</v>
+      </c>
+      <c r="F29" s="16">
+        <v>0</v>
+      </c>
+      <c r="G29" s="9">
+        <v>0</v>
+      </c>
+      <c r="H29" s="11">
+        <v>0</v>
+      </c>
+      <c r="I29" s="11">
+        <v>0</v>
+      </c>
+      <c r="J29" s="11">
+        <v>0</v>
+      </c>
+      <c r="K29" s="11">
+        <v>0</v>
+      </c>
+      <c r="L29" s="11">
+        <v>0</v>
+      </c>
+      <c r="M29" s="11">
+        <v>0</v>
+      </c>
+      <c r="N29" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" ht="18" x14ac:dyDescent="0.25">
+      <c r="A30" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B30" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="C30" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="D30" s="65">
+        <v>0</v>
+      </c>
+      <c r="E30" s="16">
+        <v>0</v>
+      </c>
+      <c r="F30" s="16">
+        <v>0</v>
+      </c>
+      <c r="G30" s="9">
+        <v>0</v>
+      </c>
+      <c r="H30" s="11">
+        <v>0</v>
+      </c>
+      <c r="I30" s="11">
+        <v>0</v>
+      </c>
+      <c r="J30" s="11">
+        <v>0</v>
+      </c>
+      <c r="K30" s="11">
+        <v>0</v>
+      </c>
+      <c r="L30" s="11">
+        <v>0</v>
+      </c>
+      <c r="M30" s="11">
+        <v>0</v>
+      </c>
+      <c r="N30" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" ht="18" x14ac:dyDescent="0.25">
+      <c r="A31" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B31" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C31" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="D31" s="65">
+        <v>0</v>
+      </c>
+      <c r="E31" s="16">
+        <v>0</v>
+      </c>
+      <c r="F31" s="16">
+        <v>0</v>
+      </c>
+      <c r="G31" s="9">
+        <v>0</v>
+      </c>
+      <c r="H31" s="11">
+        <v>0</v>
+      </c>
+      <c r="I31" s="11">
+        <v>0</v>
+      </c>
+      <c r="J31" s="11">
+        <v>0</v>
+      </c>
+      <c r="K31" s="11">
+        <v>0</v>
+      </c>
+      <c r="L31" s="11">
+        <v>0</v>
+      </c>
+      <c r="M31" s="11">
+        <v>0</v>
+      </c>
+      <c r="N31" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" ht="18" x14ac:dyDescent="0.25">
+      <c r="A32" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B32" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="C32" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="D32" s="65">
+        <v>0</v>
+      </c>
+      <c r="E32" s="16">
+        <v>0</v>
+      </c>
+      <c r="F32" s="16">
+        <v>0</v>
+      </c>
+      <c r="G32" s="9">
+        <v>0</v>
+      </c>
+      <c r="H32" s="11">
+        <v>0</v>
+      </c>
+      <c r="I32" s="11">
+        <v>0</v>
+      </c>
+      <c r="J32" s="11">
+        <v>0</v>
+      </c>
+      <c r="K32" s="11">
+        <v>0</v>
+      </c>
+      <c r="L32" s="11">
+        <v>0</v>
+      </c>
+      <c r="M32" s="11">
+        <v>0</v>
+      </c>
+      <c r="N32" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" ht="18" x14ac:dyDescent="0.25">
+      <c r="A33" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B33" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="C33" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="D33" s="65">
+        <v>0</v>
+      </c>
+      <c r="E33" s="16">
+        <v>0</v>
+      </c>
+      <c r="F33" s="16">
+        <v>0</v>
+      </c>
+      <c r="G33" s="9">
+        <v>0</v>
+      </c>
+      <c r="H33" s="11">
+        <v>0</v>
+      </c>
+      <c r="I33" s="11">
+        <v>0</v>
+      </c>
+      <c r="J33" s="11">
+        <v>0</v>
+      </c>
+      <c r="K33" s="11">
+        <v>0</v>
+      </c>
+      <c r="L33" s="11">
+        <v>0</v>
+      </c>
+      <c r="M33" s="11">
+        <v>0</v>
+      </c>
+      <c r="N33" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A34" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B34" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C34" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="D34" s="65">
+        <v>0</v>
+      </c>
+      <c r="E34" s="16">
+        <v>0</v>
+      </c>
+      <c r="F34" s="16">
+        <v>0</v>
+      </c>
+      <c r="G34" s="9">
+        <v>0</v>
+      </c>
+      <c r="H34" s="11">
+        <v>0</v>
+      </c>
+      <c r="I34" s="11">
+        <v>0</v>
+      </c>
+      <c r="J34" s="11">
+        <v>0</v>
+      </c>
+      <c r="K34" s="11">
+        <v>0</v>
+      </c>
+      <c r="L34" s="11">
+        <v>0</v>
+      </c>
+      <c r="M34" s="11">
+        <v>0</v>
+      </c>
+      <c r="N34" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A35" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="B35" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="C35" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="D35" s="65">
+        <v>0</v>
+      </c>
+      <c r="E35" s="16">
+        <v>0</v>
+      </c>
+      <c r="F35" s="16">
+        <v>0</v>
+      </c>
+      <c r="G35" s="9">
+        <v>0</v>
+      </c>
+      <c r="H35" s="11">
+        <v>0</v>
+      </c>
+      <c r="I35" s="11">
+        <v>0</v>
+      </c>
+      <c r="J35" s="11">
+        <v>0</v>
+      </c>
+      <c r="K35" s="11">
+        <v>0</v>
+      </c>
+      <c r="L35" s="11">
+        <v>0</v>
+      </c>
+      <c r="M35" s="11">
+        <v>0</v>
+      </c>
+      <c r="N35" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" ht="18" x14ac:dyDescent="0.25">
+      <c r="A36" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="B36" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C36" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="D36" s="65">
+        <v>0</v>
+      </c>
+      <c r="E36" s="16">
+        <v>0</v>
+      </c>
+      <c r="F36" s="16">
+        <v>0</v>
+      </c>
+      <c r="G36" s="9">
+        <v>0</v>
+      </c>
+      <c r="H36" s="11">
+        <v>0</v>
+      </c>
+      <c r="I36" s="11">
+        <v>0</v>
+      </c>
+      <c r="J36" s="11">
+        <v>0</v>
+      </c>
+      <c r="K36" s="11">
+        <v>0</v>
+      </c>
+      <c r="L36" s="11">
+        <v>0</v>
+      </c>
+      <c r="M36" s="11">
+        <v>0</v>
+      </c>
+      <c r="N36" s="11">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A21:E21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>